<commit_message>
Support round trip of datetime values
DateTimes are a total disaster in excel, so its pretty hacky, but
does work.

Date Times were supposed to be supported already, but obviously
I hadn't used them before and it turns out they didn't work.

Yay for testing.
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/PrimitiveLists.xlsx
+++ b/SampleTests/ExcelTests/PrimitiveLists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\SampleTests\ExcelTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1FC72F-1FEE-4345-B4C3-DCA1384C0CB9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8839F15-0D41-4F8F-919B-288A4FD8168A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{93574C7F-CD34-4A26-A791-2CAAC18DAAC8}"/>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{93574C7F-CD34-4A26-A791-2CAAC18DAAC8}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="PrimitiveLists" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <x:si>
     <x:t>Specification</x:t>
   </x:si>
@@ -106,6 +106,15 @@
   </x:si>
   <x:si>
     <x:t>StringTableSyntax_table of</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DateTimeTableSyntax_table of</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DateTime</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DateTime of</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -5826,24 +5835,24 @@
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{07917FFE-3CF1-4F24-ADDD-99FADF944328}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:dimension ref="A1:G51"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <x:selection activeCell="A25" sqref="A25"/>
+    <x:sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <x:selection activeCell="D23" sqref="D23"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <x:sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="1" width="12.54296875" style="1" customWidth="1"/>
-    <x:col min="2" max="2" width="21.08984375" style="1" customWidth="1"/>
-    <x:col min="3" max="3" width="26" style="1" bestFit="1" customWidth="1"/>
-    <x:col min="4" max="4" width="14.26953125" style="1" bestFit="1" customWidth="1"/>
+    <x:col min="1" max="1" width="12.5703125" style="1" customWidth="1"/>
+    <x:col min="2" max="2" width="21.140625" style="1" customWidth="1"/>
+    <x:col min="3" max="3" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
+    <x:col min="4" max="4" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
     <x:col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
-    <x:col min="6" max="6" width="14.26953125" style="1" bestFit="1" customWidth="1"/>
+    <x:col min="6" max="6" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
     <x:col min="7" max="7" width="60" style="1" customWidth="1"/>
-    <x:col min="8" max="8" width="36.7265625" style="1" bestFit="1" customWidth="1"/>
-    <x:col min="9" max="16384" width="9.1796875" style="1"/>
+    <x:col min="8" max="8" width="36.7109375" style="1" bestFit="1" customWidth="1"/>
+    <x:col min="9" max="16384" width="9.140625" style="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+    <x:row r="1" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -5862,7 +5871,7 @@
         <x:v>20</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <x:row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <x:c r="A3" s="1" t="s">
         <x:v>1</x:v>
       </x:c>
@@ -5870,12 +5879,12 @@
         <x:v>10</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <x:row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="B4" s="1" t="s">
         <x:v>2</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <x:row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="C5" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -5883,29 +5892,29 @@
         <x:v>11</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <x:row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <x:c r="D6" s="1" t="s">
         <x:v>2</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <x:row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="D7" s="1" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="E7"/>
       <x:c r="F7"/>
     </x:row>
-    <x:row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <x:row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="D8">
         <x:v>1</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <x:row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="D9" s="1">
         <x:v>2</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <x:row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="C10" t="s">
         <x:v>22</x:v>
       </x:c>
@@ -5913,31 +5922,31 @@
         <x:v>13</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <x:row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <x:c r="D11" s="1" t="s">
         <x:v>2</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <x:row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="D12" s="1" t="s">
         <x:v>14</x:v>
       </x:c>
       <x:c r="E12"/>
       <x:c r="F12"/>
     </x:row>
-    <x:row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <x:row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="D13">
         <x:v>1.1000000000000001</x:v>
       </x:c>
     </x:row>
-    <x:row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <x:row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="D14" s="1">
         <x:v>2.2000000000000002</x:v>
       </x:c>
       <x:c r="E14"/>
       <x:c r="F14"/>
     </x:row>
-    <x:row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <x:row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="C15" t="s">
         <x:v>23</x:v>
       </x:c>
@@ -5945,2323 +5954,2485 @@
         <x:v>15</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <x:row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <x:c r="D16" s="1" t="s">
         <x:v>2</x:v>
       </x:c>
     </x:row>
-    <x:row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <x:row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="D17" s="1" t="s">
         <x:v>16</x:v>
       </x:c>
       <x:c r="E17"/>
       <x:c r="F17"/>
     </x:row>
-    <x:row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <x:row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="D18" t="s">
         <x:v>17</x:v>
       </x:c>
     </x:row>
-    <x:row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <x:row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="D19" t="s">
         <x:v>18</x:v>
       </x:c>
     </x:row>
-    <x:row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <x:c r="C20"/>
-    </x:row>
-    <x:row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <x:c r="A21" s="1" t="s">
-        <x:v>3</x:v>
+    <x:row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="C20" t="s">
+        <x:v>24</x:v>
       </x:c>
-      <x:c r="B21" s="1" t="s">
-        <x:v>8</x:v>
+      <x:c r="D20" s="1" t="s">
+        <x:v>25</x:v>
       </x:c>
     </x:row>
-    <x:row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <x:row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <x:c r="D21" s="1" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="D22" s="1" t="s">
+        <x:v>26</x:v>
+      </x:c>
       <x:c r="E22"/>
       <x:c r="F22"/>
     </x:row>
-    <x:row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <x:c r="A23" s="1" t="s">
-        <x:v>4</x:v>
+    <x:row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="D23" s="3">
+        <x:v>36526</x:v>
       </x:c>
     </x:row>
-    <x:row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <x:c r="B24" s="1" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="C24" s="1" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D24" s="2">
-        <x:v>1</x:v>
+    <x:row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="D24" s="3">
+        <x:v>36526</x:v>
       </x:c>
       <x:c r="E24"/>
       <x:c r="F24"/>
     </x:row>
-    <x:row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <x:row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="C25"/>
     </x:row>
-    <x:row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <x:row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A26" s="1" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B26" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="E27"/>
       <x:c r="F27"/>
     </x:row>
-    <x:row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <x:c r="D29" s="2"/>
+    <x:row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A28" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
     </x:row>
-    <x:row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <x:row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="B29" s="1" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="C29" s="1" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D29" s="2">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="C30"/>
     </x:row>
-    <x:row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <x:row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="E32"/>
       <x:c r="F32"/>
     </x:row>
-    <x:row r="34" spans="3:6" x14ac:dyDescent="0.35">
+    <x:row r="34" spans="3:6" x14ac:dyDescent="0.25">
+      <x:c r="D34" s="2"/>
       <x:c r="E34"/>
       <x:c r="F34"/>
     </x:row>
-    <x:row r="35" spans="3:6" x14ac:dyDescent="0.35">
+    <x:row r="35" spans="3:6" x14ac:dyDescent="0.25">
       <x:c r="C35"/>
     </x:row>
-    <x:row r="37" spans="3:6" x14ac:dyDescent="0.35">
+    <x:row r="37" spans="3:6" x14ac:dyDescent="0.25">
       <x:c r="E37"/>
       <x:c r="F37"/>
     </x:row>
-    <x:row r="38" spans="3:6" x14ac:dyDescent="0.35">
+    <x:row r="38" spans="3:6" x14ac:dyDescent="0.25">
       <x:c r="D38" s="3"/>
     </x:row>
-    <x:row r="39" spans="3:6" x14ac:dyDescent="0.35">
+    <x:row r="39" spans="3:6" x14ac:dyDescent="0.25">
       <x:c r="D39" s="3"/>
     </x:row>
-    <x:row r="40" spans="3:6" x14ac:dyDescent="0.35">
+    <x:row r="40" spans="3:6" x14ac:dyDescent="0.25">
       <x:c r="C40"/>
     </x:row>
-    <x:row r="42" spans="3:6" x14ac:dyDescent="0.35">
+    <x:row r="42" spans="3:6" x14ac:dyDescent="0.25">
       <x:c r="E42"/>
       <x:c r="F42" s="3"/>
     </x:row>
-    <x:row r="44" spans="3:6" x14ac:dyDescent="0.35">
+    <x:row r="44" spans="3:6" x14ac:dyDescent="0.25">
       <x:c r="E44"/>
       <x:c r="F44" s="3"/>
     </x:row>
-    <x:row r="49" spans="4:4" x14ac:dyDescent="0.35">
+    <x:row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <x:c r="D49" s="2"/>
     </x:row>
-    <x:row r="51" spans="4:4" x14ac:dyDescent="0.35">
+    <x:row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <x:c r="D51" s="2"/>
     </x:row>
   </x:sheetData>
-  <x:conditionalFormatting sqref="A8:C8 A9:D9 A1:XFD4 A5:B7 G5:XFD7 E8:XFD12 A25:B25 G13:XFD44 A45:XFD1048576 A30:B44">
-    <x:cfRule type="cellIs" dxfId="675" priority="836" operator="equal">
+  <x:conditionalFormatting sqref="A8:C8 A9:D9 A1:XFD4 A5:B7 G5:XFD7 E8:XFD12 A25:B25 G13:XFD44 A45:XFD1048576 A30:B30 A35:B44">
+    <x:cfRule type="cellIs" dxfId="675" priority="940" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="674" priority="837" operator="equal">
+    <x:cfRule type="cellIs" dxfId="674" priority="941" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="673" priority="838" operator="equal">
+    <x:cfRule type="cellIs" dxfId="673" priority="942" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="672" priority="839" operator="equal">
+    <x:cfRule type="cellIs" dxfId="672" priority="943" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="671" priority="840" operator="beginsWith" text="With Properties">
+    <x:cfRule type="beginsWith" dxfId="671" priority="944" operator="beginsWith" text="With Properties">
       <x:formula>LEFT(A1,LEN("With Properties"))="With Properties"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="670" priority="841" operator="endsWith" text=" table of">
+    <x:cfRule type="endsWith" dxfId="670" priority="945" operator="endsWith" text=" table of">
       <x:formula>RIGHT(A1,LEN(" table of"))=" table of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="669" priority="842" operator="endsWith" text=" of">
+    <x:cfRule type="endsWith" dxfId="669" priority="946" operator="endsWith" text=" of">
       <x:formula>RIGHT(A1,LEN(" of"))=" of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="668" priority="843">
+    <x:cfRule type="expression" dxfId="668" priority="947">
       <x:formula>AND((RIGHT(A1048576, 3) = " of"), A2 = "With Properties")</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="667" priority="844">
+    <x:cfRule type="expression" dxfId="667" priority="948">
       <x:formula>AND(RIGHT(XFD1, 3) = " of", A2 = "With Properties")</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="A8:C8 A9:D9 A1:XFD4 A5:B7 G5:XFD7 E8:XFD12 A25:B25 G13:XFD44 A45:XFD1048576 A30:B44">
-    <x:cfRule type="notContainsBlanks" dxfId="666" priority="845">
+  <x:conditionalFormatting sqref="A8:C8 A9:D9 A1:XFD4 A5:B7 G5:XFD7 E8:XFD12 A25:B25 G13:XFD44 A45:XFD1048576 A30:B30 A35:B44">
+    <x:cfRule type="notContainsBlanks" dxfId="666" priority="949">
       <x:formula>LEN(TRIM(A1))&gt;0</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="A8:C8 A9:D9 A1:XFD4 A5:B7 G5:XFD7 E8:XFD12 A25:B25 G13:XFD44 A45:XFD1048576 A30:B44">
-    <x:cfRule type="cellIs" dxfId="665" priority="834" operator="equal">
+  <x:conditionalFormatting sqref="A8:C8 A9:D9 A1:XFD4 A5:B7 G5:XFD7 E8:XFD12 A25:B25 G13:XFD44 A45:XFD1048576 A30:B30 A35:B44">
+    <x:cfRule type="cellIs" dxfId="665" priority="938" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="664" priority="835" operator="equal">
+    <x:cfRule type="cellIs" dxfId="664" priority="939" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="A8:C8 A9:D9 A1:XFD4 A5:B7 G5:XFD7 E8:XFD12 A25:B25 G13:XFD44 A45:XFD1048576 A30:B44">
-    <x:cfRule type="cellIs" dxfId="663" priority="833" operator="equal">
+  <x:conditionalFormatting sqref="A8:C8 A9:D9 A1:XFD4 A5:B7 G5:XFD7 E8:XFD12 A25:B25 G13:XFD44 A45:XFD1048576 A30:B30 A35:B44">
+    <x:cfRule type="cellIs" dxfId="663" priority="937" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="D9">
-    <x:cfRule type="cellIs" dxfId="662" priority="823" operator="equal">
+    <x:cfRule type="cellIs" dxfId="662" priority="927" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="661" priority="824" operator="equal">
+    <x:cfRule type="cellIs" dxfId="661" priority="928" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="660" priority="825" operator="equal">
+    <x:cfRule type="cellIs" dxfId="660" priority="929" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="659" priority="826" operator="equal">
+    <x:cfRule type="cellIs" dxfId="659" priority="930" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="658" priority="827" operator="beginsWith" text="With Properties">
+    <x:cfRule type="beginsWith" dxfId="658" priority="931" operator="beginsWith" text="With Properties">
       <x:formula>LEFT(D9,LEN("With Properties"))="With Properties"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="657" priority="828" operator="endsWith" text=" table of">
+    <x:cfRule type="endsWith" dxfId="657" priority="932" operator="endsWith" text=" table of">
       <x:formula>RIGHT(D9,LEN(" table of"))=" table of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="656" priority="829" operator="endsWith" text=" of">
+    <x:cfRule type="endsWith" dxfId="656" priority="933" operator="endsWith" text=" of">
       <x:formula>RIGHT(D9,LEN(" of"))=" of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="655" priority="830">
+    <x:cfRule type="expression" dxfId="655" priority="934">
       <x:formula>AND((RIGHT(D8, 3) = " of"), D10 = "With Properties")</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="654" priority="831">
+    <x:cfRule type="expression" dxfId="654" priority="935">
       <x:formula>AND(RIGHT(C9, 3) = " of", D10 = "With Properties")</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="D9">
-    <x:cfRule type="notContainsBlanks" dxfId="653" priority="832">
+    <x:cfRule type="notContainsBlanks" dxfId="653" priority="936">
       <x:formula>LEN(TRIM(D9))&gt;0</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="D9">
-    <x:cfRule type="cellIs" dxfId="652" priority="821" operator="equal">
+    <x:cfRule type="cellIs" dxfId="652" priority="925" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="651" priority="822" operator="equal">
+    <x:cfRule type="cellIs" dxfId="651" priority="926" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="D9">
-    <x:cfRule type="cellIs" dxfId="650" priority="820" operator="equal">
+    <x:cfRule type="cellIs" dxfId="650" priority="924" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="A9:B9">
-    <x:cfRule type="cellIs" dxfId="649" priority="810" operator="equal">
+    <x:cfRule type="cellIs" dxfId="649" priority="914" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="648" priority="811" operator="equal">
+    <x:cfRule type="cellIs" dxfId="648" priority="915" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="647" priority="812" operator="equal">
+    <x:cfRule type="cellIs" dxfId="647" priority="916" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="646" priority="813" operator="equal">
+    <x:cfRule type="cellIs" dxfId="646" priority="917" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="645" priority="814" operator="beginsWith" text="With Properties">
+    <x:cfRule type="beginsWith" dxfId="645" priority="918" operator="beginsWith" text="With Properties">
       <x:formula>LEFT(A9,LEN("With Properties"))="With Properties"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="644" priority="815" operator="endsWith" text=" table of">
+    <x:cfRule type="endsWith" dxfId="644" priority="919" operator="endsWith" text=" table of">
       <x:formula>RIGHT(A9,LEN(" table of"))=" table of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="643" priority="816" operator="endsWith" text=" of">
+    <x:cfRule type="endsWith" dxfId="643" priority="920" operator="endsWith" text=" of">
       <x:formula>RIGHT(A9,LEN(" of"))=" of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="642" priority="817">
+    <x:cfRule type="expression" dxfId="642" priority="921">
       <x:formula>AND((RIGHT(A8, 3) = " of"), A10 = "With Properties")</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="641" priority="818">
+    <x:cfRule type="expression" dxfId="641" priority="922">
       <x:formula>AND(RIGHT(XFD9, 3) = " of", A10 = "With Properties")</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="A9:B9">
-    <x:cfRule type="notContainsBlanks" dxfId="640" priority="819">
+    <x:cfRule type="notContainsBlanks" dxfId="640" priority="923">
       <x:formula>LEN(TRIM(A9))&gt;0</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="A9:B9">
-    <x:cfRule type="cellIs" dxfId="639" priority="808" operator="equal">
+    <x:cfRule type="cellIs" dxfId="639" priority="912" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="638" priority="809" operator="equal">
+    <x:cfRule type="cellIs" dxfId="638" priority="913" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="A9:B9">
-    <x:cfRule type="cellIs" dxfId="637" priority="807" operator="equal">
+    <x:cfRule type="cellIs" dxfId="637" priority="911" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="D8">
-    <x:cfRule type="cellIs" dxfId="636" priority="784" operator="equal">
+    <x:cfRule type="cellIs" dxfId="636" priority="888" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="635" priority="785" operator="equal">
+    <x:cfRule type="cellIs" dxfId="635" priority="889" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="634" priority="786" operator="equal">
+    <x:cfRule type="cellIs" dxfId="634" priority="890" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="633" priority="787" operator="equal">
+    <x:cfRule type="cellIs" dxfId="633" priority="891" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="632" priority="788" operator="beginsWith" text="With Properties">
+    <x:cfRule type="beginsWith" dxfId="632" priority="892" operator="beginsWith" text="With Properties">
       <x:formula>LEFT(D8,LEN("With Properties"))="With Properties"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="631" priority="789" operator="endsWith" text=" table of">
+    <x:cfRule type="endsWith" dxfId="631" priority="893" operator="endsWith" text=" table of">
       <x:formula>RIGHT(D8,LEN(" table of"))=" table of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="630" priority="790" operator="endsWith" text=" of">
+    <x:cfRule type="endsWith" dxfId="630" priority="894" operator="endsWith" text=" of">
       <x:formula>RIGHT(D8,LEN(" of"))=" of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="629" priority="791">
+    <x:cfRule type="expression" dxfId="629" priority="895">
       <x:formula>AND((RIGHT(D7, 3) = " of"), D9 = "With Properties")</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="628" priority="792">
+    <x:cfRule type="expression" dxfId="628" priority="896">
       <x:formula>AND(RIGHT(C8, 3) = " of", D9 = "With Properties")</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="D8">
-    <x:cfRule type="notContainsBlanks" dxfId="627" priority="793">
+    <x:cfRule type="notContainsBlanks" dxfId="627" priority="897">
       <x:formula>LEN(TRIM(D8))&gt;0</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="D8">
-    <x:cfRule type="cellIs" dxfId="626" priority="782" operator="equal">
+    <x:cfRule type="cellIs" dxfId="626" priority="886" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="625" priority="783" operator="equal">
+    <x:cfRule type="cellIs" dxfId="625" priority="887" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="D8">
-    <x:cfRule type="cellIs" dxfId="624" priority="781" operator="equal">
+    <x:cfRule type="cellIs" dxfId="624" priority="885" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E8">
-    <x:cfRule type="cellIs" dxfId="623" priority="745" operator="equal">
+    <x:cfRule type="cellIs" dxfId="623" priority="849" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="622" priority="746" operator="equal">
+    <x:cfRule type="cellIs" dxfId="622" priority="850" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="621" priority="747" operator="equal">
+    <x:cfRule type="cellIs" dxfId="621" priority="851" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="620" priority="748" operator="equal">
+    <x:cfRule type="cellIs" dxfId="620" priority="852" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="619" priority="749" operator="beginsWith" text="With Properties">
+    <x:cfRule type="beginsWith" dxfId="619" priority="853" operator="beginsWith" text="With Properties">
       <x:formula>LEFT(E8,LEN("With Properties"))="With Properties"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="618" priority="750" operator="endsWith" text=" table of">
+    <x:cfRule type="endsWith" dxfId="618" priority="854" operator="endsWith" text=" table of">
       <x:formula>RIGHT(E8,LEN(" table of"))=" table of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="617" priority="751" operator="endsWith" text=" of">
+    <x:cfRule type="endsWith" dxfId="617" priority="855" operator="endsWith" text=" of">
       <x:formula>RIGHT(E8,LEN(" of"))=" of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="616" priority="752">
+    <x:cfRule type="expression" dxfId="616" priority="856">
       <x:formula>AND((RIGHT(E7, 3) = " of"), E9 = "With Properties")</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="615" priority="753">
+    <x:cfRule type="expression" dxfId="615" priority="857">
       <x:formula>AND(RIGHT(D8, 3) = " of", E9 = "With Properties")</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E8">
-    <x:cfRule type="notContainsBlanks" dxfId="614" priority="754">
+    <x:cfRule type="notContainsBlanks" dxfId="614" priority="858">
       <x:formula>LEN(TRIM(E8))&gt;0</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E8">
-    <x:cfRule type="cellIs" dxfId="613" priority="743" operator="equal">
+    <x:cfRule type="cellIs" dxfId="613" priority="847" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="612" priority="744" operator="equal">
+    <x:cfRule type="cellIs" dxfId="612" priority="848" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E8">
-    <x:cfRule type="cellIs" dxfId="611" priority="742" operator="equal">
+    <x:cfRule type="cellIs" dxfId="611" priority="846" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="C5:F7">
-    <x:cfRule type="cellIs" dxfId="610" priority="732" operator="equal">
+    <x:cfRule type="cellIs" dxfId="610" priority="836" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="609" priority="733" operator="equal">
+    <x:cfRule type="cellIs" dxfId="609" priority="837" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="608" priority="734" operator="equal">
+    <x:cfRule type="cellIs" dxfId="608" priority="838" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="607" priority="735" operator="equal">
+    <x:cfRule type="cellIs" dxfId="607" priority="839" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="606" priority="736" operator="beginsWith" text="With Properties">
+    <x:cfRule type="beginsWith" dxfId="606" priority="840" operator="beginsWith" text="With Properties">
       <x:formula>LEFT(C5,LEN("With Properties"))="With Properties"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="605" priority="737" operator="endsWith" text=" table of">
+    <x:cfRule type="endsWith" dxfId="605" priority="841" operator="endsWith" text=" table of">
       <x:formula>RIGHT(C5,LEN(" table of"))=" table of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="604" priority="738" operator="endsWith" text=" of">
+    <x:cfRule type="endsWith" dxfId="604" priority="842" operator="endsWith" text=" of">
       <x:formula>RIGHT(C5,LEN(" of"))=" of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="603" priority="739">
+    <x:cfRule type="expression" dxfId="603" priority="843">
       <x:formula>AND((RIGHT(C4, 3) = " of"), C6 = "With Properties")</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="602" priority="740">
+    <x:cfRule type="expression" dxfId="602" priority="844">
       <x:formula>AND(RIGHT(B5, 3) = " of", C6 = "With Properties")</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="C5:F7">
-    <x:cfRule type="notContainsBlanks" dxfId="601" priority="741">
+    <x:cfRule type="notContainsBlanks" dxfId="601" priority="845">
       <x:formula>LEN(TRIM(C5))&gt;0</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="C5:F7">
-    <x:cfRule type="cellIs" dxfId="600" priority="730" operator="equal">
+    <x:cfRule type="cellIs" dxfId="600" priority="834" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="599" priority="731" operator="equal">
+    <x:cfRule type="cellIs" dxfId="599" priority="835" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="C5:F7">
-    <x:cfRule type="cellIs" dxfId="598" priority="729" operator="equal">
+    <x:cfRule type="cellIs" dxfId="598" priority="833" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="D5:D6">
-    <x:cfRule type="cellIs" dxfId="597" priority="719" operator="equal">
+    <x:cfRule type="cellIs" dxfId="597" priority="823" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="596" priority="720" operator="equal">
+    <x:cfRule type="cellIs" dxfId="596" priority="824" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="595" priority="721" operator="equal">
+    <x:cfRule type="cellIs" dxfId="595" priority="825" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="594" priority="722" operator="equal">
+    <x:cfRule type="cellIs" dxfId="594" priority="826" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="593" priority="723" operator="beginsWith" text="With Properties">
+    <x:cfRule type="beginsWith" dxfId="593" priority="827" operator="beginsWith" text="With Properties">
       <x:formula>LEFT(D5,LEN("With Properties"))="With Properties"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="592" priority="724" operator="endsWith" text=" table of">
+    <x:cfRule type="endsWith" dxfId="592" priority="828" operator="endsWith" text=" table of">
       <x:formula>RIGHT(D5,LEN(" table of"))=" table of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="591" priority="725" operator="endsWith" text=" of">
+    <x:cfRule type="endsWith" dxfId="591" priority="829" operator="endsWith" text=" of">
       <x:formula>RIGHT(D5,LEN(" of"))=" of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="590" priority="726">
+    <x:cfRule type="expression" dxfId="590" priority="830">
       <x:formula>AND((RIGHT(D4, 3) = " of"), D6 = "With Properties")</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="589" priority="727">
+    <x:cfRule type="expression" dxfId="589" priority="831">
       <x:formula>AND(RIGHT(C5, 3) = " of", D6 = "With Properties")</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="D5:D6">
-    <x:cfRule type="notContainsBlanks" dxfId="588" priority="728">
+    <x:cfRule type="notContainsBlanks" dxfId="588" priority="832">
       <x:formula>LEN(TRIM(D5))&gt;0</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="D5:D6">
-    <x:cfRule type="cellIs" dxfId="587" priority="717" operator="equal">
+    <x:cfRule type="cellIs" dxfId="587" priority="821" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="586" priority="718" operator="equal">
+    <x:cfRule type="cellIs" dxfId="586" priority="822" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="D5:D6">
-    <x:cfRule type="cellIs" dxfId="585" priority="716" operator="equal">
+    <x:cfRule type="cellIs" dxfId="585" priority="820" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E13:F14">
-    <x:cfRule type="cellIs" dxfId="584" priority="706" operator="equal">
+    <x:cfRule type="cellIs" dxfId="584" priority="810" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="583" priority="707" operator="equal">
+    <x:cfRule type="cellIs" dxfId="583" priority="811" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="582" priority="708" operator="equal">
+    <x:cfRule type="cellIs" dxfId="582" priority="812" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="581" priority="709" operator="equal">
+    <x:cfRule type="cellIs" dxfId="581" priority="813" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="580" priority="710" operator="beginsWith" text="With Properties">
+    <x:cfRule type="beginsWith" dxfId="580" priority="814" operator="beginsWith" text="With Properties">
       <x:formula>LEFT(E13,LEN("With Properties"))="With Properties"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="579" priority="711" operator="endsWith" text=" table of">
+    <x:cfRule type="endsWith" dxfId="579" priority="815" operator="endsWith" text=" table of">
       <x:formula>RIGHT(E13,LEN(" table of"))=" table of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="578" priority="712" operator="endsWith" text=" of">
+    <x:cfRule type="endsWith" dxfId="578" priority="816" operator="endsWith" text=" of">
       <x:formula>RIGHT(E13,LEN(" of"))=" of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="577" priority="713">
+    <x:cfRule type="expression" dxfId="577" priority="817">
       <x:formula>AND((RIGHT(E12, 3) = " of"), E14 = "With Properties")</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="576" priority="714">
+    <x:cfRule type="expression" dxfId="576" priority="818">
       <x:formula>AND(RIGHT(D13, 3) = " of", E14 = "With Properties")</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E13:F14">
-    <x:cfRule type="notContainsBlanks" dxfId="575" priority="715">
+    <x:cfRule type="notContainsBlanks" dxfId="575" priority="819">
       <x:formula>LEN(TRIM(E13))&gt;0</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E13:F14">
-    <x:cfRule type="cellIs" dxfId="574" priority="704" operator="equal">
+    <x:cfRule type="cellIs" dxfId="574" priority="808" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="573" priority="705" operator="equal">
+    <x:cfRule type="cellIs" dxfId="573" priority="809" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E13:F14">
-    <x:cfRule type="cellIs" dxfId="572" priority="703" operator="equal">
+    <x:cfRule type="cellIs" dxfId="572" priority="807" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E18:F22">
-    <x:cfRule type="cellIs" dxfId="571" priority="680" operator="equal">
+    <x:cfRule type="cellIs" dxfId="571" priority="784" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="570" priority="681" operator="equal">
+    <x:cfRule type="cellIs" dxfId="570" priority="785" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="569" priority="682" operator="equal">
+    <x:cfRule type="cellIs" dxfId="569" priority="786" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="568" priority="683" operator="equal">
+    <x:cfRule type="cellIs" dxfId="568" priority="787" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="567" priority="684" operator="beginsWith" text="With Properties">
+    <x:cfRule type="beginsWith" dxfId="567" priority="788" operator="beginsWith" text="With Properties">
       <x:formula>LEFT(E18,LEN("With Properties"))="With Properties"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="566" priority="685" operator="endsWith" text=" table of">
+    <x:cfRule type="endsWith" dxfId="566" priority="789" operator="endsWith" text=" table of">
       <x:formula>RIGHT(E18,LEN(" table of"))=" table of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="565" priority="686" operator="endsWith" text=" of">
+    <x:cfRule type="endsWith" dxfId="565" priority="790" operator="endsWith" text=" of">
       <x:formula>RIGHT(E18,LEN(" of"))=" of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="564" priority="687">
+    <x:cfRule type="expression" dxfId="564" priority="791">
       <x:formula>AND((RIGHT(E17, 3) = " of"), E19 = "With Properties")</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="563" priority="688">
+    <x:cfRule type="expression" dxfId="563" priority="792">
       <x:formula>AND(RIGHT(D18, 3) = " of", E19 = "With Properties")</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E18:F22">
-    <x:cfRule type="notContainsBlanks" dxfId="562" priority="689">
+    <x:cfRule type="notContainsBlanks" dxfId="562" priority="793">
       <x:formula>LEN(TRIM(E18))&gt;0</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E18:F22">
-    <x:cfRule type="cellIs" dxfId="561" priority="678" operator="equal">
+    <x:cfRule type="cellIs" dxfId="561" priority="782" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="560" priority="679" operator="equal">
+    <x:cfRule type="cellIs" dxfId="560" priority="783" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E18:F22">
-    <x:cfRule type="cellIs" dxfId="559" priority="677" operator="equal">
+    <x:cfRule type="cellIs" dxfId="559" priority="781" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E18">
-    <x:cfRule type="cellIs" dxfId="558" priority="628" operator="equal">
+    <x:cfRule type="cellIs" dxfId="558" priority="732" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="557" priority="629" operator="equal">
+    <x:cfRule type="cellIs" dxfId="557" priority="733" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="556" priority="630" operator="equal">
+    <x:cfRule type="cellIs" dxfId="556" priority="734" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="555" priority="631" operator="equal">
+    <x:cfRule type="cellIs" dxfId="555" priority="735" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="554" priority="632" operator="beginsWith" text="With Properties">
+    <x:cfRule type="beginsWith" dxfId="554" priority="736" operator="beginsWith" text="With Properties">
       <x:formula>LEFT(E18,LEN("With Properties"))="With Properties"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="553" priority="633" operator="endsWith" text=" table of">
+    <x:cfRule type="endsWith" dxfId="553" priority="737" operator="endsWith" text=" table of">
       <x:formula>RIGHT(E18,LEN(" table of"))=" table of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="552" priority="634" operator="endsWith" text=" of">
+    <x:cfRule type="endsWith" dxfId="552" priority="738" operator="endsWith" text=" of">
       <x:formula>RIGHT(E18,LEN(" of"))=" of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="551" priority="635">
+    <x:cfRule type="expression" dxfId="551" priority="739">
       <x:formula>AND((RIGHT(E17, 3) = " of"), E19 = "With Properties")</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="550" priority="636">
+    <x:cfRule type="expression" dxfId="550" priority="740">
       <x:formula>AND(RIGHT(D18, 3) = " of", E19 = "With Properties")</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E18">
-    <x:cfRule type="notContainsBlanks" dxfId="549" priority="637">
+    <x:cfRule type="notContainsBlanks" dxfId="549" priority="741">
       <x:formula>LEN(TRIM(E18))&gt;0</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E18">
-    <x:cfRule type="cellIs" dxfId="548" priority="626" operator="equal">
+    <x:cfRule type="cellIs" dxfId="548" priority="730" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="547" priority="627" operator="equal">
+    <x:cfRule type="cellIs" dxfId="547" priority="731" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E18">
-    <x:cfRule type="cellIs" dxfId="546" priority="625" operator="equal">
+    <x:cfRule type="cellIs" dxfId="546" priority="729" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E15:F17">
-    <x:cfRule type="cellIs" dxfId="545" priority="615" operator="equal">
+    <x:cfRule type="cellIs" dxfId="545" priority="719" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="544" priority="616" operator="equal">
+    <x:cfRule type="cellIs" dxfId="544" priority="720" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="543" priority="617" operator="equal">
+    <x:cfRule type="cellIs" dxfId="543" priority="721" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="542" priority="618" operator="equal">
+    <x:cfRule type="cellIs" dxfId="542" priority="722" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="541" priority="619" operator="beginsWith" text="With Properties">
+    <x:cfRule type="beginsWith" dxfId="541" priority="723" operator="beginsWith" text="With Properties">
       <x:formula>LEFT(E15,LEN("With Properties"))="With Properties"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="540" priority="620" operator="endsWith" text=" table of">
+    <x:cfRule type="endsWith" dxfId="540" priority="724" operator="endsWith" text=" table of">
       <x:formula>RIGHT(E15,LEN(" table of"))=" table of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="539" priority="621" operator="endsWith" text=" of">
+    <x:cfRule type="endsWith" dxfId="539" priority="725" operator="endsWith" text=" of">
       <x:formula>RIGHT(E15,LEN(" of"))=" of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="538" priority="622">
+    <x:cfRule type="expression" dxfId="538" priority="726">
       <x:formula>AND((RIGHT(E14, 3) = " of"), E16 = "With Properties")</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="537" priority="623">
+    <x:cfRule type="expression" dxfId="537" priority="727">
       <x:formula>AND(RIGHT(D15, 3) = " of", E16 = "With Properties")</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E15:F17">
-    <x:cfRule type="notContainsBlanks" dxfId="536" priority="624">
+    <x:cfRule type="notContainsBlanks" dxfId="536" priority="728">
       <x:formula>LEN(TRIM(E15))&gt;0</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E15:F17">
-    <x:cfRule type="cellIs" dxfId="535" priority="613" operator="equal">
+    <x:cfRule type="cellIs" dxfId="535" priority="717" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="534" priority="614" operator="equal">
+    <x:cfRule type="cellIs" dxfId="534" priority="718" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E15:F17">
-    <x:cfRule type="cellIs" dxfId="533" priority="612" operator="equal">
+    <x:cfRule type="cellIs" dxfId="533" priority="716" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E23:F24">
-    <x:cfRule type="cellIs" dxfId="532" priority="589" operator="equal">
+    <x:cfRule type="cellIs" dxfId="532" priority="693" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="531" priority="590" operator="equal">
+    <x:cfRule type="cellIs" dxfId="531" priority="694" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="530" priority="591" operator="equal">
+    <x:cfRule type="cellIs" dxfId="530" priority="695" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="529" priority="592" operator="equal">
+    <x:cfRule type="cellIs" dxfId="529" priority="696" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="528" priority="593" operator="beginsWith" text="With Properties">
+    <x:cfRule type="beginsWith" dxfId="528" priority="697" operator="beginsWith" text="With Properties">
       <x:formula>LEFT(E23,LEN("With Properties"))="With Properties"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="527" priority="594" operator="endsWith" text=" table of">
+    <x:cfRule type="endsWith" dxfId="527" priority="698" operator="endsWith" text=" table of">
       <x:formula>RIGHT(E23,LEN(" table of"))=" table of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="526" priority="595" operator="endsWith" text=" of">
+    <x:cfRule type="endsWith" dxfId="526" priority="699" operator="endsWith" text=" of">
       <x:formula>RIGHT(E23,LEN(" of"))=" of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="525" priority="596">
+    <x:cfRule type="expression" dxfId="525" priority="700">
       <x:formula>AND((RIGHT(E22, 3) = " of"), E24 = "With Properties")</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="524" priority="597">
+    <x:cfRule type="expression" dxfId="524" priority="701">
       <x:formula>AND(RIGHT(D23, 3) = " of", E24 = "With Properties")</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E23:F24">
-    <x:cfRule type="notContainsBlanks" dxfId="523" priority="598">
+    <x:cfRule type="notContainsBlanks" dxfId="523" priority="702">
       <x:formula>LEN(TRIM(E23))&gt;0</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E23:F24">
-    <x:cfRule type="cellIs" dxfId="522" priority="587" operator="equal">
+    <x:cfRule type="cellIs" dxfId="522" priority="691" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="521" priority="588" operator="equal">
+    <x:cfRule type="cellIs" dxfId="521" priority="692" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E23:F24">
-    <x:cfRule type="cellIs" dxfId="520" priority="586" operator="equal">
+    <x:cfRule type="cellIs" dxfId="520" priority="690" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C30:F31 E28:F29 C33:C34 C32:E32">
-    <x:cfRule type="cellIs" dxfId="519" priority="563" operator="equal">
+  <x:conditionalFormatting sqref="C30:F30 E28:F29 E32 E31:F31">
+    <x:cfRule type="cellIs" dxfId="519" priority="667" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="518" priority="564" operator="equal">
+    <x:cfRule type="cellIs" dxfId="518" priority="668" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="517" priority="565" operator="equal">
+    <x:cfRule type="cellIs" dxfId="517" priority="669" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="516" priority="566" operator="equal">
+    <x:cfRule type="cellIs" dxfId="516" priority="670" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="515" priority="567" operator="beginsWith" text="With Properties">
+    <x:cfRule type="beginsWith" dxfId="515" priority="671" operator="beginsWith" text="With Properties">
       <x:formula>LEFT(C28,LEN("With Properties"))="With Properties"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="514" priority="568" operator="endsWith" text=" table of">
+    <x:cfRule type="endsWith" dxfId="514" priority="672" operator="endsWith" text=" table of">
       <x:formula>RIGHT(C28,LEN(" table of"))=" table of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="513" priority="569" operator="endsWith" text=" of">
+    <x:cfRule type="endsWith" dxfId="513" priority="673" operator="endsWith" text=" of">
       <x:formula>RIGHT(C28,LEN(" of"))=" of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="512" priority="570">
+    <x:cfRule type="expression" dxfId="512" priority="674">
       <x:formula>AND((RIGHT(C27, 3) = " of"), C29 = "With Properties")</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="511" priority="571">
+    <x:cfRule type="expression" dxfId="511" priority="675">
       <x:formula>AND(RIGHT(B28, 3) = " of", C29 = "With Properties")</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C30:F31 E28:F29 C33:C34 C32:E32">
-    <x:cfRule type="notContainsBlanks" dxfId="510" priority="572">
+  <x:conditionalFormatting sqref="C30:F30 E28:F29 E32 E31:F31">
+    <x:cfRule type="notContainsBlanks" dxfId="510" priority="676">
       <x:formula>LEN(TRIM(C28))&gt;0</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C30:F31 E28:F29 C33:C34 C32:E32">
-    <x:cfRule type="cellIs" dxfId="509" priority="561" operator="equal">
+  <x:conditionalFormatting sqref="C30:F30 E28:F29 E32 E31:F31">
+    <x:cfRule type="cellIs" dxfId="509" priority="665" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="508" priority="562" operator="equal">
+    <x:cfRule type="cellIs" dxfId="508" priority="666" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C30:F31 E28:F29 C33:C34 C32:E32">
-    <x:cfRule type="cellIs" dxfId="507" priority="560" operator="equal">
+  <x:conditionalFormatting sqref="C30:F30 E28:F29 E32 E31:F31">
+    <x:cfRule type="cellIs" dxfId="507" priority="664" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D30:D31">
-    <x:cfRule type="cellIs" dxfId="506" priority="537" operator="equal">
+  <x:conditionalFormatting sqref="D30">
+    <x:cfRule type="cellIs" dxfId="506" priority="641" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="505" priority="538" operator="equal">
+    <x:cfRule type="cellIs" dxfId="505" priority="642" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="504" priority="539" operator="equal">
+    <x:cfRule type="cellIs" dxfId="504" priority="643" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="503" priority="540" operator="equal">
+    <x:cfRule type="cellIs" dxfId="503" priority="644" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="502" priority="541" operator="beginsWith" text="With Properties">
+    <x:cfRule type="beginsWith" dxfId="502" priority="645" operator="beginsWith" text="With Properties">
       <x:formula>LEFT(D30,LEN("With Properties"))="With Properties"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="501" priority="542" operator="endsWith" text=" table of">
+    <x:cfRule type="endsWith" dxfId="501" priority="646" operator="endsWith" text=" table of">
       <x:formula>RIGHT(D30,LEN(" table of"))=" table of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="500" priority="543" operator="endsWith" text=" of">
+    <x:cfRule type="endsWith" dxfId="500" priority="647" operator="endsWith" text=" of">
       <x:formula>RIGHT(D30,LEN(" of"))=" of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="499" priority="544">
+    <x:cfRule type="expression" dxfId="499" priority="648">
       <x:formula>AND((RIGHT(D29, 3) = " of"), D31 = "With Properties")</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="498" priority="545">
+    <x:cfRule type="expression" dxfId="498" priority="649">
       <x:formula>AND(RIGHT(C30, 3) = " of", D31 = "With Properties")</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D30:D31">
-    <x:cfRule type="notContainsBlanks" dxfId="497" priority="546">
+  <x:conditionalFormatting sqref="D30">
+    <x:cfRule type="notContainsBlanks" dxfId="497" priority="650">
       <x:formula>LEN(TRIM(D30))&gt;0</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D30:D31">
-    <x:cfRule type="cellIs" dxfId="496" priority="535" operator="equal">
+  <x:conditionalFormatting sqref="D30">
+    <x:cfRule type="cellIs" dxfId="496" priority="639" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="495" priority="536" operator="equal">
+    <x:cfRule type="cellIs" dxfId="495" priority="640" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D30:D31">
-    <x:cfRule type="cellIs" dxfId="494" priority="534" operator="equal">
+  <x:conditionalFormatting sqref="D30">
+    <x:cfRule type="cellIs" dxfId="494" priority="638" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E28">
-    <x:cfRule type="cellIs" dxfId="493" priority="511" operator="equal">
+    <x:cfRule type="cellIs" dxfId="493" priority="615" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="492" priority="512" operator="equal">
+    <x:cfRule type="cellIs" dxfId="492" priority="616" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="491" priority="513" operator="equal">
+    <x:cfRule type="cellIs" dxfId="491" priority="617" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="490" priority="514" operator="equal">
+    <x:cfRule type="cellIs" dxfId="490" priority="618" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="489" priority="515" operator="beginsWith" text="With Properties">
+    <x:cfRule type="beginsWith" dxfId="489" priority="619" operator="beginsWith" text="With Properties">
       <x:formula>LEFT(E28,LEN("With Properties"))="With Properties"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="488" priority="516" operator="endsWith" text=" table of">
+    <x:cfRule type="endsWith" dxfId="488" priority="620" operator="endsWith" text=" table of">
       <x:formula>RIGHT(E28,LEN(" table of"))=" table of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="487" priority="517" operator="endsWith" text=" of">
+    <x:cfRule type="endsWith" dxfId="487" priority="621" operator="endsWith" text=" of">
       <x:formula>RIGHT(E28,LEN(" of"))=" of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="486" priority="518">
+    <x:cfRule type="expression" dxfId="486" priority="622">
       <x:formula>AND((RIGHT(E27, 3) = " of"), E29 = "With Properties")</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="485" priority="519">
+    <x:cfRule type="expression" dxfId="485" priority="623">
       <x:formula>AND(RIGHT(D28, 3) = " of", E29 = "With Properties")</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E28">
-    <x:cfRule type="notContainsBlanks" dxfId="484" priority="520">
+    <x:cfRule type="notContainsBlanks" dxfId="484" priority="624">
       <x:formula>LEN(TRIM(E28))&gt;0</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E28">
-    <x:cfRule type="cellIs" dxfId="483" priority="509" operator="equal">
+    <x:cfRule type="cellIs" dxfId="483" priority="613" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="482" priority="510" operator="equal">
+    <x:cfRule type="cellIs" dxfId="482" priority="614" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E28">
-    <x:cfRule type="cellIs" dxfId="481" priority="508" operator="equal">
+    <x:cfRule type="cellIs" dxfId="481" priority="612" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="C25:F25 E26:F27">
-    <x:cfRule type="cellIs" dxfId="480" priority="498" operator="equal">
+    <x:cfRule type="cellIs" dxfId="480" priority="602" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="479" priority="499" operator="equal">
+    <x:cfRule type="cellIs" dxfId="479" priority="603" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="478" priority="500" operator="equal">
+    <x:cfRule type="cellIs" dxfId="478" priority="604" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="477" priority="501" operator="equal">
+    <x:cfRule type="cellIs" dxfId="477" priority="605" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="476" priority="502" operator="beginsWith" text="With Properties">
+    <x:cfRule type="beginsWith" dxfId="476" priority="606" operator="beginsWith" text="With Properties">
       <x:formula>LEFT(C25,LEN("With Properties"))="With Properties"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="475" priority="503" operator="endsWith" text=" table of">
+    <x:cfRule type="endsWith" dxfId="475" priority="607" operator="endsWith" text=" table of">
       <x:formula>RIGHT(C25,LEN(" table of"))=" table of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="474" priority="504" operator="endsWith" text=" of">
+    <x:cfRule type="endsWith" dxfId="474" priority="608" operator="endsWith" text=" of">
       <x:formula>RIGHT(C25,LEN(" of"))=" of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="473" priority="505">
+    <x:cfRule type="expression" dxfId="473" priority="609">
       <x:formula>AND((RIGHT(C24, 3) = " of"), C26 = "With Properties")</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="472" priority="506">
+    <x:cfRule type="expression" dxfId="472" priority="610">
       <x:formula>AND(RIGHT(B25, 3) = " of", C26 = "With Properties")</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="C25:F25 E26:F27">
-    <x:cfRule type="notContainsBlanks" dxfId="471" priority="507">
+    <x:cfRule type="notContainsBlanks" dxfId="471" priority="611">
       <x:formula>LEN(TRIM(C25))&gt;0</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="C25:F25 E26:F27">
-    <x:cfRule type="cellIs" dxfId="470" priority="496" operator="equal">
+    <x:cfRule type="cellIs" dxfId="470" priority="600" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="469" priority="497" operator="equal">
+    <x:cfRule type="cellIs" dxfId="469" priority="601" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="C25:F25 E26:F27">
-    <x:cfRule type="cellIs" dxfId="468" priority="495" operator="equal">
+    <x:cfRule type="cellIs" dxfId="468" priority="599" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="D25">
-    <x:cfRule type="cellIs" dxfId="467" priority="485" operator="equal">
+    <x:cfRule type="cellIs" dxfId="467" priority="589" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="466" priority="486" operator="equal">
+    <x:cfRule type="cellIs" dxfId="466" priority="590" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="465" priority="487" operator="equal">
+    <x:cfRule type="cellIs" dxfId="465" priority="591" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="464" priority="488" operator="equal">
+    <x:cfRule type="cellIs" dxfId="464" priority="592" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="463" priority="489" operator="beginsWith" text="With Properties">
+    <x:cfRule type="beginsWith" dxfId="463" priority="593" operator="beginsWith" text="With Properties">
       <x:formula>LEFT(D25,LEN("With Properties"))="With Properties"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="462" priority="490" operator="endsWith" text=" table of">
+    <x:cfRule type="endsWith" dxfId="462" priority="594" operator="endsWith" text=" table of">
       <x:formula>RIGHT(D25,LEN(" table of"))=" table of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="461" priority="491" operator="endsWith" text=" of">
+    <x:cfRule type="endsWith" dxfId="461" priority="595" operator="endsWith" text=" of">
       <x:formula>RIGHT(D25,LEN(" of"))=" of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="460" priority="492">
+    <x:cfRule type="expression" dxfId="460" priority="596">
       <x:formula>AND((RIGHT(D24, 3) = " of"), D26 = "With Properties")</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="459" priority="493">
+    <x:cfRule type="expression" dxfId="459" priority="597">
       <x:formula>AND(RIGHT(C25, 3) = " of", D26 = "With Properties")</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="D25">
-    <x:cfRule type="notContainsBlanks" dxfId="458" priority="494">
+    <x:cfRule type="notContainsBlanks" dxfId="458" priority="598">
       <x:formula>LEN(TRIM(D25))&gt;0</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="D25">
-    <x:cfRule type="cellIs" dxfId="457" priority="483" operator="equal">
+    <x:cfRule type="cellIs" dxfId="457" priority="587" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="456" priority="484" operator="equal">
+    <x:cfRule type="cellIs" dxfId="456" priority="588" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="D25">
-    <x:cfRule type="cellIs" dxfId="455" priority="482" operator="equal">
+    <x:cfRule type="cellIs" dxfId="455" priority="586" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D33:F33 D34:E34">
-    <x:cfRule type="cellIs" dxfId="454" priority="472" operator="equal">
+  <x:conditionalFormatting sqref="E33:F33 E34">
+    <x:cfRule type="cellIs" dxfId="454" priority="576" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="453" priority="473" operator="equal">
+    <x:cfRule type="cellIs" dxfId="453" priority="577" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="452" priority="474" operator="equal">
+    <x:cfRule type="cellIs" dxfId="452" priority="578" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="451" priority="475" operator="equal">
+    <x:cfRule type="cellIs" dxfId="451" priority="579" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="450" priority="476" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(D33,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="449" priority="477" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(D33,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="448" priority="478" operator="endsWith" text=" of">
-      <x:formula>RIGHT(D33,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="447" priority="479">
-      <x:formula>AND((RIGHT(D32, 3) = " of"), D34 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="446" priority="480">
-      <x:formula>AND(RIGHT(C33, 3) = " of", D34 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D33:F33 D34:E34">
-    <x:cfRule type="notContainsBlanks" dxfId="445" priority="481">
-      <x:formula>LEN(TRIM(D33))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D33:F33 D34:E34">
-    <x:cfRule type="cellIs" dxfId="444" priority="470" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="450" priority="580" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(E33,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="449" priority="581" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(E33,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="448" priority="582" operator="endsWith" text=" of">
+      <x:formula>RIGHT(E33,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="447" priority="583">
+      <x:formula>AND((RIGHT(E32, 3) = " of"), E34 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="446" priority="584">
+      <x:formula>AND(RIGHT(D33, 3) = " of", E34 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="E33:F33 E34">
+    <x:cfRule type="notContainsBlanks" dxfId="445" priority="585">
+      <x:formula>LEN(TRIM(E33))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="E33:F33 E34">
+    <x:cfRule type="cellIs" dxfId="444" priority="574" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="443" priority="471" operator="equal">
+    <x:cfRule type="cellIs" dxfId="443" priority="575" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D33:F33 D34:E34">
-    <x:cfRule type="cellIs" dxfId="442" priority="469" operator="equal">
+  <x:conditionalFormatting sqref="E33:F33 E34">
+    <x:cfRule type="cellIs" dxfId="442" priority="573" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D33">
-    <x:cfRule type="cellIs" dxfId="441" priority="459" operator="equal">
+  <x:conditionalFormatting sqref="F32">
+    <x:cfRule type="cellIs" dxfId="441" priority="537" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="440" priority="460" operator="equal">
+    <x:cfRule type="cellIs" dxfId="440" priority="538" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="439" priority="461" operator="equal">
+    <x:cfRule type="cellIs" dxfId="439" priority="539" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="438" priority="462" operator="equal">
+    <x:cfRule type="cellIs" dxfId="438" priority="540" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="437" priority="463" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(D33,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="436" priority="464" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(D33,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="435" priority="465" operator="endsWith" text=" of">
-      <x:formula>RIGHT(D33,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="434" priority="466">
-      <x:formula>AND((RIGHT(D32, 3) = " of"), D34 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="433" priority="467">
-      <x:formula>AND(RIGHT(C33, 3) = " of", D34 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D33">
-    <x:cfRule type="notContainsBlanks" dxfId="432" priority="468">
-      <x:formula>LEN(TRIM(D33))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D33">
-    <x:cfRule type="cellIs" dxfId="431" priority="457" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="437" priority="541" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(F32,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="436" priority="542" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(F32,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="435" priority="543" operator="endsWith" text=" of">
+      <x:formula>RIGHT(F32,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="434" priority="544">
+      <x:formula>AND((RIGHT(F31, 3) = " of"), F33 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="433" priority="545">
+      <x:formula>AND(RIGHT(E32, 3) = " of", F33 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="F32">
+    <x:cfRule type="notContainsBlanks" dxfId="432" priority="546">
+      <x:formula>LEN(TRIM(F32))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="F32">
+    <x:cfRule type="cellIs" dxfId="431" priority="535" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="430" priority="458" operator="equal">
+    <x:cfRule type="cellIs" dxfId="430" priority="536" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D33">
-    <x:cfRule type="cellIs" dxfId="429" priority="456" operator="equal">
+  <x:conditionalFormatting sqref="F32">
+    <x:cfRule type="cellIs" dxfId="429" priority="534" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="F32">
-    <x:cfRule type="cellIs" dxfId="428" priority="433" operator="equal">
+  <x:conditionalFormatting sqref="F34">
+    <x:cfRule type="cellIs" dxfId="428" priority="524" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="427" priority="434" operator="equal">
+    <x:cfRule type="cellIs" dxfId="427" priority="525" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="426" priority="435" operator="equal">
+    <x:cfRule type="cellIs" dxfId="426" priority="526" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="425" priority="436" operator="equal">
+    <x:cfRule type="cellIs" dxfId="425" priority="527" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="424" priority="437" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(F32,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="423" priority="438" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(F32,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="422" priority="439" operator="endsWith" text=" of">
-      <x:formula>RIGHT(F32,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="421" priority="440">
-      <x:formula>AND((RIGHT(F31, 3) = " of"), F33 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="420" priority="441">
-      <x:formula>AND(RIGHT(E32, 3) = " of", F33 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="F32">
-    <x:cfRule type="notContainsBlanks" dxfId="419" priority="442">
-      <x:formula>LEN(TRIM(F32))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="F32">
-    <x:cfRule type="cellIs" dxfId="418" priority="431" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="424" priority="528" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(F34,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="423" priority="529" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(F34,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="422" priority="530" operator="endsWith" text=" of">
+      <x:formula>RIGHT(F34,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="421" priority="531">
+      <x:formula>AND((RIGHT(F33, 3) = " of"), F35 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="420" priority="532">
+      <x:formula>AND(RIGHT(E34, 3) = " of", F35 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="F34">
+    <x:cfRule type="notContainsBlanks" dxfId="419" priority="533">
+      <x:formula>LEN(TRIM(F34))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="F34">
+    <x:cfRule type="cellIs" dxfId="418" priority="522" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="417" priority="432" operator="equal">
+    <x:cfRule type="cellIs" dxfId="417" priority="523" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="F32">
-    <x:cfRule type="cellIs" dxfId="416" priority="430" operator="equal">
+  <x:conditionalFormatting sqref="F34">
+    <x:cfRule type="cellIs" dxfId="416" priority="521" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="F34">
-    <x:cfRule type="cellIs" dxfId="415" priority="420" operator="equal">
+  <x:conditionalFormatting sqref="C38:C39 C40:F41 E38:F39 C43:C44 C42:E42">
+    <x:cfRule type="cellIs" dxfId="415" priority="511" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="414" priority="421" operator="equal">
+    <x:cfRule type="cellIs" dxfId="414" priority="512" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="413" priority="422" operator="equal">
+    <x:cfRule type="cellIs" dxfId="413" priority="513" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="412" priority="423" operator="equal">
+    <x:cfRule type="cellIs" dxfId="412" priority="514" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="411" priority="424" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(F34,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="410" priority="425" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(F34,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="409" priority="426" operator="endsWith" text=" of">
-      <x:formula>RIGHT(F34,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="408" priority="427">
-      <x:formula>AND((RIGHT(F33, 3) = " of"), F35 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="407" priority="428">
-      <x:formula>AND(RIGHT(E34, 3) = " of", F35 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="F34">
-    <x:cfRule type="notContainsBlanks" dxfId="406" priority="429">
-      <x:formula>LEN(TRIM(F34))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="F34">
-    <x:cfRule type="cellIs" dxfId="405" priority="418" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="411" priority="515" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(C38,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="410" priority="516" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(C38,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="409" priority="517" operator="endsWith" text=" of">
+      <x:formula>RIGHT(C38,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="408" priority="518">
+      <x:formula>AND((RIGHT(C37, 3) = " of"), C39 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="407" priority="519">
+      <x:formula>AND(RIGHT(B38, 3) = " of", C39 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="C38:C39 C40:F41 E38:F39 C43:C44 C42:E42">
+    <x:cfRule type="notContainsBlanks" dxfId="406" priority="520">
+      <x:formula>LEN(TRIM(C38))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="C38:C39 C40:F41 E38:F39 C43:C44 C42:E42">
+    <x:cfRule type="cellIs" dxfId="405" priority="509" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="404" priority="419" operator="equal">
+    <x:cfRule type="cellIs" dxfId="404" priority="510" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="F34">
-    <x:cfRule type="cellIs" dxfId="403" priority="417" operator="equal">
+  <x:conditionalFormatting sqref="C38:C39 C40:F41 E38:F39 C43:C44 C42:E42">
+    <x:cfRule type="cellIs" dxfId="403" priority="508" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C38:C39 C40:F41 E38:F39 C43:C44 C42:E42">
-    <x:cfRule type="cellIs" dxfId="402" priority="407" operator="equal">
+  <x:conditionalFormatting sqref="D40:D41">
+    <x:cfRule type="cellIs" dxfId="402" priority="485" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="401" priority="408" operator="equal">
+    <x:cfRule type="cellIs" dxfId="401" priority="486" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="400" priority="409" operator="equal">
+    <x:cfRule type="cellIs" dxfId="400" priority="487" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="399" priority="410" operator="equal">
+    <x:cfRule type="cellIs" dxfId="399" priority="488" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="398" priority="411" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(C38,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="397" priority="412" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(C38,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="396" priority="413" operator="endsWith" text=" of">
-      <x:formula>RIGHT(C38,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="395" priority="414">
-      <x:formula>AND((RIGHT(C37, 3) = " of"), C39 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="394" priority="415">
-      <x:formula>AND(RIGHT(B38, 3) = " of", C39 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C38:C39 C40:F41 E38:F39 C43:C44 C42:E42">
-    <x:cfRule type="notContainsBlanks" dxfId="393" priority="416">
-      <x:formula>LEN(TRIM(C38))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C38:C39 C40:F41 E38:F39 C43:C44 C42:E42">
-    <x:cfRule type="cellIs" dxfId="392" priority="405" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="398" priority="489" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(D40,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="397" priority="490" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(D40,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="396" priority="491" operator="endsWith" text=" of">
+      <x:formula>RIGHT(D40,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="395" priority="492">
+      <x:formula>AND((RIGHT(D39, 3) = " of"), D41 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="394" priority="493">
+      <x:formula>AND(RIGHT(C40, 3) = " of", D41 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D40:D41">
+    <x:cfRule type="notContainsBlanks" dxfId="393" priority="494">
+      <x:formula>LEN(TRIM(D40))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D40:D41">
+    <x:cfRule type="cellIs" dxfId="392" priority="483" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="391" priority="406" operator="equal">
+    <x:cfRule type="cellIs" dxfId="391" priority="484" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C38:C39 C40:F41 E38:F39 C43:C44 C42:E42">
-    <x:cfRule type="cellIs" dxfId="390" priority="404" operator="equal">
+  <x:conditionalFormatting sqref="D40:D41">
+    <x:cfRule type="cellIs" dxfId="390" priority="482" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D40:D41">
-    <x:cfRule type="cellIs" dxfId="389" priority="381" operator="equal">
+  <x:conditionalFormatting sqref="D38">
+    <x:cfRule type="cellIs" dxfId="389" priority="472" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="388" priority="382" operator="equal">
+    <x:cfRule type="cellIs" dxfId="388" priority="473" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="387" priority="383" operator="equal">
+    <x:cfRule type="cellIs" dxfId="387" priority="474" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="386" priority="384" operator="equal">
+    <x:cfRule type="cellIs" dxfId="386" priority="475" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="385" priority="385" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(D40,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="384" priority="386" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(D40,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="383" priority="387" operator="endsWith" text=" of">
-      <x:formula>RIGHT(D40,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="382" priority="388">
-      <x:formula>AND((RIGHT(D39, 3) = " of"), D41 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="381" priority="389">
-      <x:formula>AND(RIGHT(C40, 3) = " of", D41 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D40:D41">
-    <x:cfRule type="notContainsBlanks" dxfId="380" priority="390">
-      <x:formula>LEN(TRIM(D40))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D40:D41">
-    <x:cfRule type="cellIs" dxfId="379" priority="379" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="385" priority="476" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(D38,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="384" priority="477" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(D38,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="383" priority="478" operator="endsWith" text=" of">
+      <x:formula>RIGHT(D38,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="382" priority="479">
+      <x:formula>AND((RIGHT(D37, 3) = " of"), D39 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="381" priority="480">
+      <x:formula>AND(RIGHT(C38, 3) = " of", D39 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D38">
+    <x:cfRule type="notContainsBlanks" dxfId="380" priority="481">
+      <x:formula>LEN(TRIM(D38))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D38">
+    <x:cfRule type="cellIs" dxfId="379" priority="470" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="378" priority="380" operator="equal">
+    <x:cfRule type="cellIs" dxfId="378" priority="471" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D40:D41">
-    <x:cfRule type="cellIs" dxfId="377" priority="378" operator="equal">
+  <x:conditionalFormatting sqref="D38">
+    <x:cfRule type="cellIs" dxfId="377" priority="469" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D38">
-    <x:cfRule type="cellIs" dxfId="376" priority="368" operator="equal">
+  <x:conditionalFormatting sqref="E38">
+    <x:cfRule type="cellIs" dxfId="376" priority="459" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="375" priority="369" operator="equal">
+    <x:cfRule type="cellIs" dxfId="375" priority="460" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="374" priority="370" operator="equal">
+    <x:cfRule type="cellIs" dxfId="374" priority="461" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="373" priority="371" operator="equal">
+    <x:cfRule type="cellIs" dxfId="373" priority="462" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="372" priority="372" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(D38,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="371" priority="373" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(D38,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="370" priority="374" operator="endsWith" text=" of">
-      <x:formula>RIGHT(D38,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="369" priority="375">
-      <x:formula>AND((RIGHT(D37, 3) = " of"), D39 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="368" priority="376">
-      <x:formula>AND(RIGHT(C38, 3) = " of", D39 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D38">
-    <x:cfRule type="notContainsBlanks" dxfId="367" priority="377">
-      <x:formula>LEN(TRIM(D38))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D38">
-    <x:cfRule type="cellIs" dxfId="366" priority="366" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="372" priority="463" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(E38,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="371" priority="464" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(E38,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="370" priority="465" operator="endsWith" text=" of">
+      <x:formula>RIGHT(E38,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="369" priority="466">
+      <x:formula>AND((RIGHT(E37, 3) = " of"), E39 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="368" priority="467">
+      <x:formula>AND(RIGHT(D38, 3) = " of", E39 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="E38">
+    <x:cfRule type="notContainsBlanks" dxfId="367" priority="468">
+      <x:formula>LEN(TRIM(E38))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="E38">
+    <x:cfRule type="cellIs" dxfId="366" priority="457" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="365" priority="367" operator="equal">
+    <x:cfRule type="cellIs" dxfId="365" priority="458" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D38">
-    <x:cfRule type="cellIs" dxfId="364" priority="365" operator="equal">
+  <x:conditionalFormatting sqref="E38">
+    <x:cfRule type="cellIs" dxfId="364" priority="456" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="E38">
-    <x:cfRule type="cellIs" dxfId="363" priority="355" operator="equal">
+  <x:conditionalFormatting sqref="C35:F37">
+    <x:cfRule type="cellIs" dxfId="363" priority="446" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="362" priority="356" operator="equal">
+    <x:cfRule type="cellIs" dxfId="362" priority="447" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="361" priority="357" operator="equal">
+    <x:cfRule type="cellIs" dxfId="361" priority="448" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="360" priority="358" operator="equal">
+    <x:cfRule type="cellIs" dxfId="360" priority="449" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="359" priority="359" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(E38,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="358" priority="360" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(E38,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="357" priority="361" operator="endsWith" text=" of">
-      <x:formula>RIGHT(E38,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="356" priority="362">
-      <x:formula>AND((RIGHT(E37, 3) = " of"), E39 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="355" priority="363">
-      <x:formula>AND(RIGHT(D38, 3) = " of", E39 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="E38">
-    <x:cfRule type="notContainsBlanks" dxfId="354" priority="364">
-      <x:formula>LEN(TRIM(E38))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="E38">
-    <x:cfRule type="cellIs" dxfId="353" priority="353" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="359" priority="450" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(C35,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="358" priority="451" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(C35,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="357" priority="452" operator="endsWith" text=" of">
+      <x:formula>RIGHT(C35,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="356" priority="453">
+      <x:formula>AND((RIGHT(C34, 3) = " of"), C36 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="355" priority="454">
+      <x:formula>AND(RIGHT(B35, 3) = " of", C36 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="C35:F37">
+    <x:cfRule type="notContainsBlanks" dxfId="354" priority="455">
+      <x:formula>LEN(TRIM(C35))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="C35:F37">
+    <x:cfRule type="cellIs" dxfId="353" priority="444" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="352" priority="354" operator="equal">
+    <x:cfRule type="cellIs" dxfId="352" priority="445" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="E38">
-    <x:cfRule type="cellIs" dxfId="351" priority="352" operator="equal">
+  <x:conditionalFormatting sqref="C35:F37">
+    <x:cfRule type="cellIs" dxfId="351" priority="443" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C35:F37">
-    <x:cfRule type="cellIs" dxfId="350" priority="342" operator="equal">
+  <x:conditionalFormatting sqref="D35:D36">
+    <x:cfRule type="cellIs" dxfId="350" priority="433" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="349" priority="343" operator="equal">
+    <x:cfRule type="cellIs" dxfId="349" priority="434" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="348" priority="344" operator="equal">
+    <x:cfRule type="cellIs" dxfId="348" priority="435" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="347" priority="345" operator="equal">
+    <x:cfRule type="cellIs" dxfId="347" priority="436" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="346" priority="346" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(C35,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="345" priority="347" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(C35,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="344" priority="348" operator="endsWith" text=" of">
-      <x:formula>RIGHT(C35,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="343" priority="349">
-      <x:formula>AND((RIGHT(C34, 3) = " of"), C36 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="342" priority="350">
-      <x:formula>AND(RIGHT(B35, 3) = " of", C36 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C35:F37">
-    <x:cfRule type="notContainsBlanks" dxfId="341" priority="351">
-      <x:formula>LEN(TRIM(C35))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C35:F37">
-    <x:cfRule type="cellIs" dxfId="340" priority="340" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="346" priority="437" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(D35,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="345" priority="438" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(D35,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="344" priority="439" operator="endsWith" text=" of">
+      <x:formula>RIGHT(D35,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="343" priority="440">
+      <x:formula>AND((RIGHT(D34, 3) = " of"), D36 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="342" priority="441">
+      <x:formula>AND(RIGHT(C35, 3) = " of", D36 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D35:D36">
+    <x:cfRule type="notContainsBlanks" dxfId="341" priority="442">
+      <x:formula>LEN(TRIM(D35))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D35:D36">
+    <x:cfRule type="cellIs" dxfId="340" priority="431" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="339" priority="341" operator="equal">
+    <x:cfRule type="cellIs" dxfId="339" priority="432" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C35:F37">
-    <x:cfRule type="cellIs" dxfId="338" priority="339" operator="equal">
+  <x:conditionalFormatting sqref="D35:D36">
+    <x:cfRule type="cellIs" dxfId="338" priority="430" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D35:D36">
-    <x:cfRule type="cellIs" dxfId="337" priority="329" operator="equal">
+  <x:conditionalFormatting sqref="D43:F43 D44:E44">
+    <x:cfRule type="cellIs" dxfId="337" priority="420" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="336" priority="330" operator="equal">
+    <x:cfRule type="cellIs" dxfId="336" priority="421" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="335" priority="331" operator="equal">
+    <x:cfRule type="cellIs" dxfId="335" priority="422" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="334" priority="332" operator="equal">
+    <x:cfRule type="cellIs" dxfId="334" priority="423" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="333" priority="333" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(D35,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="332" priority="334" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(D35,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="331" priority="335" operator="endsWith" text=" of">
-      <x:formula>RIGHT(D35,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="330" priority="336">
-      <x:formula>AND((RIGHT(D34, 3) = " of"), D36 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="329" priority="337">
-      <x:formula>AND(RIGHT(C35, 3) = " of", D36 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D35:D36">
-    <x:cfRule type="notContainsBlanks" dxfId="328" priority="338">
-      <x:formula>LEN(TRIM(D35))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D35:D36">
-    <x:cfRule type="cellIs" dxfId="327" priority="327" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="333" priority="424" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(D43,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="332" priority="425" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(D43,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="331" priority="426" operator="endsWith" text=" of">
+      <x:formula>RIGHT(D43,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="330" priority="427">
+      <x:formula>AND((RIGHT(D42, 3) = " of"), D44 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="329" priority="428">
+      <x:formula>AND(RIGHT(C43, 3) = " of", D44 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D43:F43 D44:E44">
+    <x:cfRule type="notContainsBlanks" dxfId="328" priority="429">
+      <x:formula>LEN(TRIM(D43))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D43:F43 D44:E44">
+    <x:cfRule type="cellIs" dxfId="327" priority="418" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="326" priority="328" operator="equal">
+    <x:cfRule type="cellIs" dxfId="326" priority="419" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D35:D36">
-    <x:cfRule type="cellIs" dxfId="325" priority="326" operator="equal">
+  <x:conditionalFormatting sqref="D43:F43 D44:E44">
+    <x:cfRule type="cellIs" dxfId="325" priority="417" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D43:F43 D44:E44">
-    <x:cfRule type="cellIs" dxfId="324" priority="316" operator="equal">
+  <x:conditionalFormatting sqref="D43">
+    <x:cfRule type="cellIs" dxfId="324" priority="407" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="323" priority="317" operator="equal">
+    <x:cfRule type="cellIs" dxfId="323" priority="408" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="322" priority="318" operator="equal">
+    <x:cfRule type="cellIs" dxfId="322" priority="409" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="321" priority="319" operator="equal">
+    <x:cfRule type="cellIs" dxfId="321" priority="410" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="320" priority="320" operator="beginsWith" text="With Properties">
+    <x:cfRule type="beginsWith" dxfId="320" priority="411" operator="beginsWith" text="With Properties">
       <x:formula>LEFT(D43,LEN("With Properties"))="With Properties"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="319" priority="321" operator="endsWith" text=" table of">
+    <x:cfRule type="endsWith" dxfId="319" priority="412" operator="endsWith" text=" table of">
       <x:formula>RIGHT(D43,LEN(" table of"))=" table of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="318" priority="322" operator="endsWith" text=" of">
+    <x:cfRule type="endsWith" dxfId="318" priority="413" operator="endsWith" text=" of">
       <x:formula>RIGHT(D43,LEN(" of"))=" of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="317" priority="323">
+    <x:cfRule type="expression" dxfId="317" priority="414">
       <x:formula>AND((RIGHT(D42, 3) = " of"), D44 = "With Properties")</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="316" priority="324">
+    <x:cfRule type="expression" dxfId="316" priority="415">
       <x:formula>AND(RIGHT(C43, 3) = " of", D44 = "With Properties")</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D43:F43 D44:E44">
-    <x:cfRule type="notContainsBlanks" dxfId="315" priority="325">
+  <x:conditionalFormatting sqref="D43">
+    <x:cfRule type="notContainsBlanks" dxfId="315" priority="416">
       <x:formula>LEN(TRIM(D43))&gt;0</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D43:F43 D44:E44">
-    <x:cfRule type="cellIs" dxfId="314" priority="314" operator="equal">
+  <x:conditionalFormatting sqref="D43">
+    <x:cfRule type="cellIs" dxfId="314" priority="405" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="313" priority="315" operator="equal">
+    <x:cfRule type="cellIs" dxfId="313" priority="406" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D43:F43 D44:E44">
-    <x:cfRule type="cellIs" dxfId="312" priority="313" operator="equal">
+  <x:conditionalFormatting sqref="D43">
+    <x:cfRule type="cellIs" dxfId="312" priority="404" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D43">
-    <x:cfRule type="cellIs" dxfId="311" priority="303" operator="equal">
+  <x:conditionalFormatting sqref="D39">
+    <x:cfRule type="cellIs" dxfId="311" priority="394" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="310" priority="304" operator="equal">
+    <x:cfRule type="cellIs" dxfId="310" priority="395" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="309" priority="305" operator="equal">
+    <x:cfRule type="cellIs" dxfId="309" priority="396" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="308" priority="306" operator="equal">
+    <x:cfRule type="cellIs" dxfId="308" priority="397" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="307" priority="307" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(D43,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="306" priority="308" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(D43,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="305" priority="309" operator="endsWith" text=" of">
-      <x:formula>RIGHT(D43,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="304" priority="310">
-      <x:formula>AND((RIGHT(D42, 3) = " of"), D44 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="303" priority="311">
-      <x:formula>AND(RIGHT(C43, 3) = " of", D44 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D43">
-    <x:cfRule type="notContainsBlanks" dxfId="302" priority="312">
-      <x:formula>LEN(TRIM(D43))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D43">
-    <x:cfRule type="cellIs" dxfId="301" priority="301" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="307" priority="398" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(D39,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="306" priority="399" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(D39,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="305" priority="400" operator="endsWith" text=" of">
+      <x:formula>RIGHT(D39,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="304" priority="401">
+      <x:formula>AND((RIGHT(D38, 3) = " of"), D40 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="303" priority="402">
+      <x:formula>AND(RIGHT(C39, 3) = " of", D40 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D39">
+    <x:cfRule type="notContainsBlanks" dxfId="302" priority="403">
+      <x:formula>LEN(TRIM(D39))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D39">
+    <x:cfRule type="cellIs" dxfId="301" priority="392" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="300" priority="302" operator="equal">
+    <x:cfRule type="cellIs" dxfId="300" priority="393" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D43">
-    <x:cfRule type="cellIs" dxfId="299" priority="300" operator="equal">
+  <x:conditionalFormatting sqref="D39">
+    <x:cfRule type="cellIs" dxfId="299" priority="391" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D39">
-    <x:cfRule type="cellIs" dxfId="298" priority="290" operator="equal">
+  <x:conditionalFormatting sqref="F42">
+    <x:cfRule type="cellIs" dxfId="298" priority="381" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="297" priority="291" operator="equal">
+    <x:cfRule type="cellIs" dxfId="297" priority="382" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="296" priority="292" operator="equal">
+    <x:cfRule type="cellIs" dxfId="296" priority="383" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="295" priority="293" operator="equal">
+    <x:cfRule type="cellIs" dxfId="295" priority="384" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="294" priority="294" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(D39,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="293" priority="295" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(D39,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="292" priority="296" operator="endsWith" text=" of">
-      <x:formula>RIGHT(D39,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="291" priority="297">
-      <x:formula>AND((RIGHT(D38, 3) = " of"), D40 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="290" priority="298">
-      <x:formula>AND(RIGHT(C39, 3) = " of", D40 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D39">
-    <x:cfRule type="notContainsBlanks" dxfId="289" priority="299">
-      <x:formula>LEN(TRIM(D39))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D39">
-    <x:cfRule type="cellIs" dxfId="288" priority="288" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="294" priority="385" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(F42,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="293" priority="386" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(F42,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="292" priority="387" operator="endsWith" text=" of">
+      <x:formula>RIGHT(F42,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="291" priority="388">
+      <x:formula>AND((RIGHT(F41, 3) = " of"), F43 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="290" priority="389">
+      <x:formula>AND(RIGHT(E42, 3) = " of", F43 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="F42">
+    <x:cfRule type="notContainsBlanks" dxfId="289" priority="390">
+      <x:formula>LEN(TRIM(F42))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="F42">
+    <x:cfRule type="cellIs" dxfId="288" priority="379" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="287" priority="289" operator="equal">
+    <x:cfRule type="cellIs" dxfId="287" priority="380" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D39">
-    <x:cfRule type="cellIs" dxfId="286" priority="287" operator="equal">
+  <x:conditionalFormatting sqref="F42">
+    <x:cfRule type="cellIs" dxfId="286" priority="378" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="F42">
-    <x:cfRule type="cellIs" dxfId="285" priority="277" operator="equal">
+  <x:conditionalFormatting sqref="F44">
+    <x:cfRule type="cellIs" dxfId="285" priority="368" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="284" priority="278" operator="equal">
+    <x:cfRule type="cellIs" dxfId="284" priority="369" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="283" priority="279" operator="equal">
+    <x:cfRule type="cellIs" dxfId="283" priority="370" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="282" priority="280" operator="equal">
+    <x:cfRule type="cellIs" dxfId="282" priority="371" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="281" priority="281" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(F42,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="280" priority="282" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(F42,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="279" priority="283" operator="endsWith" text=" of">
-      <x:formula>RIGHT(F42,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="278" priority="284">
-      <x:formula>AND((RIGHT(F41, 3) = " of"), F43 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="277" priority="285">
-      <x:formula>AND(RIGHT(E42, 3) = " of", F43 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="F42">
-    <x:cfRule type="notContainsBlanks" dxfId="276" priority="286">
-      <x:formula>LEN(TRIM(F42))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="F42">
-    <x:cfRule type="cellIs" dxfId="275" priority="275" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="281" priority="372" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(F44,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="280" priority="373" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(F44,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="279" priority="374" operator="endsWith" text=" of">
+      <x:formula>RIGHT(F44,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="278" priority="375">
+      <x:formula>AND((RIGHT(F43, 3) = " of"), F45 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="277" priority="376">
+      <x:formula>AND(RIGHT(E44, 3) = " of", F45 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="F44">
+    <x:cfRule type="notContainsBlanks" dxfId="276" priority="377">
+      <x:formula>LEN(TRIM(F44))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="F44">
+    <x:cfRule type="cellIs" dxfId="275" priority="366" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="274" priority="276" operator="equal">
+    <x:cfRule type="cellIs" dxfId="274" priority="367" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="F42">
-    <x:cfRule type="cellIs" dxfId="273" priority="274" operator="equal">
+  <x:conditionalFormatting sqref="F44">
+    <x:cfRule type="cellIs" dxfId="273" priority="365" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="F44">
-    <x:cfRule type="cellIs" dxfId="272" priority="264" operator="equal">
+  <x:conditionalFormatting sqref="A10:B14">
+    <x:cfRule type="cellIs" dxfId="272" priority="355" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="271" priority="265" operator="equal">
+    <x:cfRule type="cellIs" dxfId="271" priority="356" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="270" priority="266" operator="equal">
+    <x:cfRule type="cellIs" dxfId="270" priority="357" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="269" priority="267" operator="equal">
+    <x:cfRule type="cellIs" dxfId="269" priority="358" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="268" priority="268" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(F44,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="267" priority="269" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(F44,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="266" priority="270" operator="endsWith" text=" of">
-      <x:formula>RIGHT(F44,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="265" priority="271">
-      <x:formula>AND((RIGHT(F43, 3) = " of"), F45 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="264" priority="272">
-      <x:formula>AND(RIGHT(E44, 3) = " of", F45 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="F44">
-    <x:cfRule type="notContainsBlanks" dxfId="263" priority="273">
-      <x:formula>LEN(TRIM(F44))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="F44">
-    <x:cfRule type="cellIs" dxfId="262" priority="262" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="268" priority="359" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(A10,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="267" priority="360" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(A10,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="266" priority="361" operator="endsWith" text=" of">
+      <x:formula>RIGHT(A10,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="265" priority="362">
+      <x:formula>AND((RIGHT(A9, 3) = " of"), A11 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="264" priority="363">
+      <x:formula>AND(RIGHT(XFD10, 3) = " of", A11 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="A10:B14">
+    <x:cfRule type="notContainsBlanks" dxfId="263" priority="364">
+      <x:formula>LEN(TRIM(A10))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="A10:B14">
+    <x:cfRule type="cellIs" dxfId="262" priority="353" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="261" priority="263" operator="equal">
+    <x:cfRule type="cellIs" dxfId="261" priority="354" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="F44">
-    <x:cfRule type="cellIs" dxfId="260" priority="261" operator="equal">
+  <x:conditionalFormatting sqref="A10:B14">
+    <x:cfRule type="cellIs" dxfId="260" priority="352" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="A10:B14">
-    <x:cfRule type="cellIs" dxfId="259" priority="251" operator="equal">
+  <x:conditionalFormatting sqref="C13 C14:D14">
+    <x:cfRule type="cellIs" dxfId="259" priority="342" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="258" priority="252" operator="equal">
+    <x:cfRule type="cellIs" dxfId="258" priority="343" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="257" priority="253" operator="equal">
+    <x:cfRule type="cellIs" dxfId="257" priority="344" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="256" priority="254" operator="equal">
+    <x:cfRule type="cellIs" dxfId="256" priority="345" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="255" priority="255" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(A10,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="254" priority="256" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(A10,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="253" priority="257" operator="endsWith" text=" of">
-      <x:formula>RIGHT(A10,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="252" priority="258">
-      <x:formula>AND((RIGHT(A9, 3) = " of"), A11 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="251" priority="259">
-      <x:formula>AND(RIGHT(XFD10, 3) = " of", A11 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="A10:B14">
-    <x:cfRule type="notContainsBlanks" dxfId="250" priority="260">
-      <x:formula>LEN(TRIM(A10))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="A10:B14">
-    <x:cfRule type="cellIs" dxfId="249" priority="249" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="255" priority="346" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(C13,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="254" priority="347" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(C13,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="253" priority="348" operator="endsWith" text=" of">
+      <x:formula>RIGHT(C13,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="252" priority="349">
+      <x:formula>AND((RIGHT(C12, 3) = " of"), C14 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="251" priority="350">
+      <x:formula>AND(RIGHT(B13, 3) = " of", C14 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="C13 C14:D14">
+    <x:cfRule type="notContainsBlanks" dxfId="250" priority="351">
+      <x:formula>LEN(TRIM(C13))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="C13 C14:D14">
+    <x:cfRule type="cellIs" dxfId="249" priority="340" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="248" priority="250" operator="equal">
+    <x:cfRule type="cellIs" dxfId="248" priority="341" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="A10:B14">
-    <x:cfRule type="cellIs" dxfId="247" priority="248" operator="equal">
+  <x:conditionalFormatting sqref="C13 C14:D14">
+    <x:cfRule type="cellIs" dxfId="247" priority="339" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C13 C14:D14">
-    <x:cfRule type="cellIs" dxfId="246" priority="238" operator="equal">
+  <x:conditionalFormatting sqref="D14">
+    <x:cfRule type="cellIs" dxfId="246" priority="329" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="245" priority="239" operator="equal">
+    <x:cfRule type="cellIs" dxfId="245" priority="330" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="244" priority="240" operator="equal">
+    <x:cfRule type="cellIs" dxfId="244" priority="331" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="243" priority="241" operator="equal">
+    <x:cfRule type="cellIs" dxfId="243" priority="332" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="242" priority="242" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(C13,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="241" priority="243" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(C13,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="240" priority="244" operator="endsWith" text=" of">
-      <x:formula>RIGHT(C13,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="239" priority="245">
-      <x:formula>AND((RIGHT(C12, 3) = " of"), C14 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="238" priority="246">
-      <x:formula>AND(RIGHT(B13, 3) = " of", C14 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C13 C14:D14">
-    <x:cfRule type="notContainsBlanks" dxfId="237" priority="247">
-      <x:formula>LEN(TRIM(C13))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C13 C14:D14">
-    <x:cfRule type="cellIs" dxfId="236" priority="236" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="242" priority="333" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(D14,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="241" priority="334" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(D14,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="240" priority="335" operator="endsWith" text=" of">
+      <x:formula>RIGHT(D14,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="239" priority="336">
+      <x:formula>AND((RIGHT(D13, 3) = " of"), D15 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="238" priority="337">
+      <x:formula>AND(RIGHT(C14, 3) = " of", D15 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D14">
+    <x:cfRule type="notContainsBlanks" dxfId="237" priority="338">
+      <x:formula>LEN(TRIM(D14))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D14">
+    <x:cfRule type="cellIs" dxfId="236" priority="327" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="235" priority="237" operator="equal">
+    <x:cfRule type="cellIs" dxfId="235" priority="328" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C13 C14:D14">
-    <x:cfRule type="cellIs" dxfId="234" priority="235" operator="equal">
+  <x:conditionalFormatting sqref="D14">
+    <x:cfRule type="cellIs" dxfId="234" priority="326" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D14">
-    <x:cfRule type="cellIs" dxfId="233" priority="225" operator="equal">
+  <x:conditionalFormatting sqref="D13">
+    <x:cfRule type="cellIs" dxfId="233" priority="316" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="232" priority="226" operator="equal">
+    <x:cfRule type="cellIs" dxfId="232" priority="317" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="231" priority="227" operator="equal">
+    <x:cfRule type="cellIs" dxfId="231" priority="318" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="230" priority="228" operator="equal">
+    <x:cfRule type="cellIs" dxfId="230" priority="319" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="229" priority="229" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(D14,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="228" priority="230" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(D14,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="227" priority="231" operator="endsWith" text=" of">
-      <x:formula>RIGHT(D14,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="226" priority="232">
-      <x:formula>AND((RIGHT(D13, 3) = " of"), D15 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="225" priority="233">
-      <x:formula>AND(RIGHT(C14, 3) = " of", D15 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D14">
-    <x:cfRule type="notContainsBlanks" dxfId="224" priority="234">
-      <x:formula>LEN(TRIM(D14))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D14">
-    <x:cfRule type="cellIs" dxfId="223" priority="223" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="229" priority="320" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(D13,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="228" priority="321" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(D13,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="227" priority="322" operator="endsWith" text=" of">
+      <x:formula>RIGHT(D13,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="226" priority="323">
+      <x:formula>AND((RIGHT(D12, 3) = " of"), D14 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="225" priority="324">
+      <x:formula>AND(RIGHT(C13, 3) = " of", D14 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D13">
+    <x:cfRule type="notContainsBlanks" dxfId="224" priority="325">
+      <x:formula>LEN(TRIM(D13))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D13">
+    <x:cfRule type="cellIs" dxfId="223" priority="314" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="222" priority="224" operator="equal">
+    <x:cfRule type="cellIs" dxfId="222" priority="315" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D14">
-    <x:cfRule type="cellIs" dxfId="221" priority="222" operator="equal">
+  <x:conditionalFormatting sqref="D13">
+    <x:cfRule type="cellIs" dxfId="221" priority="313" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D13">
-    <x:cfRule type="cellIs" dxfId="220" priority="212" operator="equal">
+  <x:conditionalFormatting sqref="C10:D12">
+    <x:cfRule type="cellIs" dxfId="220" priority="303" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="219" priority="213" operator="equal">
+    <x:cfRule type="cellIs" dxfId="219" priority="304" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="218" priority="214" operator="equal">
+    <x:cfRule type="cellIs" dxfId="218" priority="305" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="217" priority="215" operator="equal">
+    <x:cfRule type="cellIs" dxfId="217" priority="306" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="216" priority="216" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(D13,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="215" priority="217" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(D13,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="214" priority="218" operator="endsWith" text=" of">
-      <x:formula>RIGHT(D13,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="213" priority="219">
-      <x:formula>AND((RIGHT(D12, 3) = " of"), D14 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="212" priority="220">
-      <x:formula>AND(RIGHT(C13, 3) = " of", D14 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D13">
-    <x:cfRule type="notContainsBlanks" dxfId="211" priority="221">
-      <x:formula>LEN(TRIM(D13))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D13">
-    <x:cfRule type="cellIs" dxfId="210" priority="210" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="216" priority="307" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(C10,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="215" priority="308" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(C10,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="214" priority="309" operator="endsWith" text=" of">
+      <x:formula>RIGHT(C10,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="213" priority="310">
+      <x:formula>AND((RIGHT(C9, 3) = " of"), C11 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="212" priority="311">
+      <x:formula>AND(RIGHT(B10, 3) = " of", C11 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="C10:D12">
+    <x:cfRule type="notContainsBlanks" dxfId="211" priority="312">
+      <x:formula>LEN(TRIM(C10))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="C10:D12">
+    <x:cfRule type="cellIs" dxfId="210" priority="301" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="209" priority="211" operator="equal">
+    <x:cfRule type="cellIs" dxfId="209" priority="302" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D13">
-    <x:cfRule type="cellIs" dxfId="208" priority="209" operator="equal">
+  <x:conditionalFormatting sqref="C10:D12">
+    <x:cfRule type="cellIs" dxfId="208" priority="300" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C10:D12">
-    <x:cfRule type="cellIs" dxfId="207" priority="199" operator="equal">
+  <x:conditionalFormatting sqref="D10:D11">
+    <x:cfRule type="cellIs" dxfId="207" priority="290" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="206" priority="200" operator="equal">
+    <x:cfRule type="cellIs" dxfId="206" priority="291" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="205" priority="201" operator="equal">
+    <x:cfRule type="cellIs" dxfId="205" priority="292" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="204" priority="202" operator="equal">
+    <x:cfRule type="cellIs" dxfId="204" priority="293" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="203" priority="203" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(C10,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="202" priority="204" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(C10,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="201" priority="205" operator="endsWith" text=" of">
-      <x:formula>RIGHT(C10,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="200" priority="206">
-      <x:formula>AND((RIGHT(C9, 3) = " of"), C11 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="199" priority="207">
-      <x:formula>AND(RIGHT(B10, 3) = " of", C11 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C10:D12">
-    <x:cfRule type="notContainsBlanks" dxfId="198" priority="208">
-      <x:formula>LEN(TRIM(C10))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C10:D12">
-    <x:cfRule type="cellIs" dxfId="197" priority="197" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="203" priority="294" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(D10,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="202" priority="295" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(D10,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="201" priority="296" operator="endsWith" text=" of">
+      <x:formula>RIGHT(D10,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="200" priority="297">
+      <x:formula>AND((RIGHT(D9, 3) = " of"), D11 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="199" priority="298">
+      <x:formula>AND(RIGHT(C10, 3) = " of", D11 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D10:D11">
+    <x:cfRule type="notContainsBlanks" dxfId="198" priority="299">
+      <x:formula>LEN(TRIM(D10))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D10:D11">
+    <x:cfRule type="cellIs" dxfId="197" priority="288" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="196" priority="198" operator="equal">
+    <x:cfRule type="cellIs" dxfId="196" priority="289" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C10:D12">
-    <x:cfRule type="cellIs" dxfId="195" priority="196" operator="equal">
+  <x:conditionalFormatting sqref="D10:D11">
+    <x:cfRule type="cellIs" dxfId="195" priority="287" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D10:D11">
-    <x:cfRule type="cellIs" dxfId="194" priority="186" operator="equal">
+  <x:conditionalFormatting sqref="A15:B19">
+    <x:cfRule type="cellIs" dxfId="194" priority="277" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="193" priority="187" operator="equal">
+    <x:cfRule type="cellIs" dxfId="193" priority="278" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="192" priority="188" operator="equal">
+    <x:cfRule type="cellIs" dxfId="192" priority="279" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="191" priority="189" operator="equal">
+    <x:cfRule type="cellIs" dxfId="191" priority="280" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="190" priority="190" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(D10,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="189" priority="191" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(D10,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="188" priority="192" operator="endsWith" text=" of">
-      <x:formula>RIGHT(D10,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="187" priority="193">
-      <x:formula>AND((RIGHT(D9, 3) = " of"), D11 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="186" priority="194">
-      <x:formula>AND(RIGHT(C10, 3) = " of", D11 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D10:D11">
-    <x:cfRule type="notContainsBlanks" dxfId="185" priority="195">
-      <x:formula>LEN(TRIM(D10))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D10:D11">
-    <x:cfRule type="cellIs" dxfId="184" priority="184" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="190" priority="281" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(A15,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="189" priority="282" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(A15,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="188" priority="283" operator="endsWith" text=" of">
+      <x:formula>RIGHT(A15,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="187" priority="284">
+      <x:formula>AND((RIGHT(A14, 3) = " of"), A16 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="186" priority="285">
+      <x:formula>AND(RIGHT(XFD15, 3) = " of", A16 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="A15:B19">
+    <x:cfRule type="notContainsBlanks" dxfId="185" priority="286">
+      <x:formula>LEN(TRIM(A15))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="A15:B19">
+    <x:cfRule type="cellIs" dxfId="184" priority="275" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="183" priority="185" operator="equal">
+    <x:cfRule type="cellIs" dxfId="183" priority="276" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D10:D11">
-    <x:cfRule type="cellIs" dxfId="182" priority="183" operator="equal">
+  <x:conditionalFormatting sqref="A15:B19">
+    <x:cfRule type="cellIs" dxfId="182" priority="274" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="A15:B19">
-    <x:cfRule type="cellIs" dxfId="181" priority="173" operator="equal">
+  <x:conditionalFormatting sqref="C18:C19">
+    <x:cfRule type="cellIs" dxfId="181" priority="264" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="180" priority="174" operator="equal">
+    <x:cfRule type="cellIs" dxfId="180" priority="265" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="179" priority="175" operator="equal">
+    <x:cfRule type="cellIs" dxfId="179" priority="266" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="178" priority="176" operator="equal">
+    <x:cfRule type="cellIs" dxfId="178" priority="267" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="177" priority="177" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(A15,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="176" priority="178" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(A15,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="175" priority="179" operator="endsWith" text=" of">
-      <x:formula>RIGHT(A15,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="174" priority="180">
-      <x:formula>AND((RIGHT(A14, 3) = " of"), A16 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="173" priority="181">
-      <x:formula>AND(RIGHT(XFD15, 3) = " of", A16 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="A15:B19">
-    <x:cfRule type="notContainsBlanks" dxfId="172" priority="182">
-      <x:formula>LEN(TRIM(A15))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="A15:B19">
-    <x:cfRule type="cellIs" dxfId="171" priority="171" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="177" priority="268" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(C18,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="176" priority="269" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(C18,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="175" priority="270" operator="endsWith" text=" of">
+      <x:formula>RIGHT(C18,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="174" priority="271">
+      <x:formula>AND((RIGHT(C17, 3) = " of"), C19 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="173" priority="272">
+      <x:formula>AND(RIGHT(B18, 3) = " of", C19 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="C18:C19">
+    <x:cfRule type="notContainsBlanks" dxfId="172" priority="273">
+      <x:formula>LEN(TRIM(C18))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="C18:C19">
+    <x:cfRule type="cellIs" dxfId="171" priority="262" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="170" priority="172" operator="equal">
+    <x:cfRule type="cellIs" dxfId="170" priority="263" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="A15:B19">
-    <x:cfRule type="cellIs" dxfId="169" priority="170" operator="equal">
+  <x:conditionalFormatting sqref="C18:C19">
+    <x:cfRule type="cellIs" dxfId="169" priority="261" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C18:C19">
-    <x:cfRule type="cellIs" dxfId="168" priority="160" operator="equal">
+  <x:conditionalFormatting sqref="D18">
+    <x:cfRule type="cellIs" dxfId="168" priority="251" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="167" priority="161" operator="equal">
+    <x:cfRule type="cellIs" dxfId="167" priority="252" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="166" priority="162" operator="equal">
+    <x:cfRule type="cellIs" dxfId="166" priority="253" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="165" priority="163" operator="equal">
+    <x:cfRule type="cellIs" dxfId="165" priority="254" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="164" priority="164" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(C18,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="163" priority="165" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(C18,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="162" priority="166" operator="endsWith" text=" of">
-      <x:formula>RIGHT(C18,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="161" priority="167">
-      <x:formula>AND((RIGHT(C17, 3) = " of"), C19 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="160" priority="168">
-      <x:formula>AND(RIGHT(B18, 3) = " of", C19 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C18:C19">
-    <x:cfRule type="notContainsBlanks" dxfId="159" priority="169">
-      <x:formula>LEN(TRIM(C18))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C18:C19">
-    <x:cfRule type="cellIs" dxfId="158" priority="158" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="164" priority="255" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(D18,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="163" priority="256" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(D18,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="162" priority="257" operator="endsWith" text=" of">
+      <x:formula>RIGHT(D18,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="161" priority="258">
+      <x:formula>AND((RIGHT(D17, 3) = " of"), D19 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="160" priority="259">
+      <x:formula>AND(RIGHT(C18, 3) = " of", D19 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D18">
+    <x:cfRule type="notContainsBlanks" dxfId="159" priority="260">
+      <x:formula>LEN(TRIM(D18))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D18">
+    <x:cfRule type="cellIs" dxfId="158" priority="249" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="157" priority="159" operator="equal">
+    <x:cfRule type="cellIs" dxfId="157" priority="250" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C18:C19">
-    <x:cfRule type="cellIs" dxfId="156" priority="157" operator="equal">
+  <x:conditionalFormatting sqref="D18">
+    <x:cfRule type="cellIs" dxfId="156" priority="248" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D18">
-    <x:cfRule type="cellIs" dxfId="155" priority="147" operator="equal">
+  <x:conditionalFormatting sqref="C15:D17">
+    <x:cfRule type="cellIs" dxfId="155" priority="238" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="154" priority="148" operator="equal">
+    <x:cfRule type="cellIs" dxfId="154" priority="239" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="153" priority="149" operator="equal">
+    <x:cfRule type="cellIs" dxfId="153" priority="240" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="152" priority="150" operator="equal">
+    <x:cfRule type="cellIs" dxfId="152" priority="241" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="151" priority="151" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(D18,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="150" priority="152" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(D18,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="149" priority="153" operator="endsWith" text=" of">
-      <x:formula>RIGHT(D18,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="148" priority="154">
-      <x:formula>AND((RIGHT(D17, 3) = " of"), D19 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="147" priority="155">
-      <x:formula>AND(RIGHT(C18, 3) = " of", D19 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D18">
-    <x:cfRule type="notContainsBlanks" dxfId="146" priority="156">
-      <x:formula>LEN(TRIM(D18))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D18">
-    <x:cfRule type="cellIs" dxfId="145" priority="145" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="151" priority="242" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(C15,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="150" priority="243" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(C15,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="149" priority="244" operator="endsWith" text=" of">
+      <x:formula>RIGHT(C15,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="148" priority="245">
+      <x:formula>AND((RIGHT(C14, 3) = " of"), C16 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="147" priority="246">
+      <x:formula>AND(RIGHT(B15, 3) = " of", C16 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="C15:D17">
+    <x:cfRule type="notContainsBlanks" dxfId="146" priority="247">
+      <x:formula>LEN(TRIM(C15))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="C15:D17">
+    <x:cfRule type="cellIs" dxfId="145" priority="236" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="144" priority="146" operator="equal">
+    <x:cfRule type="cellIs" dxfId="144" priority="237" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D18">
-    <x:cfRule type="cellIs" dxfId="143" priority="144" operator="equal">
+  <x:conditionalFormatting sqref="C15:D17">
+    <x:cfRule type="cellIs" dxfId="143" priority="235" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C15:D17">
-    <x:cfRule type="cellIs" dxfId="142" priority="134" operator="equal">
+  <x:conditionalFormatting sqref="D15:D16">
+    <x:cfRule type="cellIs" dxfId="142" priority="225" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="141" priority="135" operator="equal">
+    <x:cfRule type="cellIs" dxfId="141" priority="226" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="140" priority="136" operator="equal">
+    <x:cfRule type="cellIs" dxfId="140" priority="227" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="139" priority="137" operator="equal">
+    <x:cfRule type="cellIs" dxfId="139" priority="228" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="138" priority="138" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(C15,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="137" priority="139" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(C15,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="136" priority="140" operator="endsWith" text=" of">
-      <x:formula>RIGHT(C15,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="135" priority="141">
-      <x:formula>AND((RIGHT(C14, 3) = " of"), C16 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="134" priority="142">
-      <x:formula>AND(RIGHT(B15, 3) = " of", C16 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C15:D17">
-    <x:cfRule type="notContainsBlanks" dxfId="133" priority="143">
-      <x:formula>LEN(TRIM(C15))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C15:D17">
-    <x:cfRule type="cellIs" dxfId="132" priority="132" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="138" priority="229" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(D15,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="137" priority="230" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(D15,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="136" priority="231" operator="endsWith" text=" of">
+      <x:formula>RIGHT(D15,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="135" priority="232">
+      <x:formula>AND((RIGHT(D14, 3) = " of"), D16 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="134" priority="233">
+      <x:formula>AND(RIGHT(C15, 3) = " of", D16 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D15:D16">
+    <x:cfRule type="notContainsBlanks" dxfId="133" priority="234">
+      <x:formula>LEN(TRIM(D15))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D15:D16">
+    <x:cfRule type="cellIs" dxfId="132" priority="223" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="131" priority="133" operator="equal">
+    <x:cfRule type="cellIs" dxfId="131" priority="224" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C15:D17">
-    <x:cfRule type="cellIs" dxfId="130" priority="131" operator="equal">
+  <x:conditionalFormatting sqref="D15:D16">
+    <x:cfRule type="cellIs" dxfId="130" priority="222" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D15:D16">
-    <x:cfRule type="cellIs" dxfId="129" priority="121" operator="equal">
+  <x:conditionalFormatting sqref="D19">
+    <x:cfRule type="cellIs" dxfId="129" priority="212" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="128" priority="122" operator="equal">
+    <x:cfRule type="cellIs" dxfId="128" priority="213" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="127" priority="123" operator="equal">
+    <x:cfRule type="cellIs" dxfId="127" priority="214" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="126" priority="124" operator="equal">
+    <x:cfRule type="cellIs" dxfId="126" priority="215" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="125" priority="125" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(D15,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="124" priority="126" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(D15,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="123" priority="127" operator="endsWith" text=" of">
-      <x:formula>RIGHT(D15,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="122" priority="128">
-      <x:formula>AND((RIGHT(D14, 3) = " of"), D16 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="121" priority="129">
-      <x:formula>AND(RIGHT(C15, 3) = " of", D16 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D15:D16">
-    <x:cfRule type="notContainsBlanks" dxfId="120" priority="130">
-      <x:formula>LEN(TRIM(D15))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D15:D16">
-    <x:cfRule type="cellIs" dxfId="119" priority="119" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="125" priority="216" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(D19,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="124" priority="217" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(D19,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="123" priority="218" operator="endsWith" text=" of">
+      <x:formula>RIGHT(D19,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="122" priority="219">
+      <x:formula>AND((RIGHT(D18, 3) = " of"), D20 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="121" priority="220">
+      <x:formula>AND(RIGHT(C19, 3) = " of", D20 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D19">
+    <x:cfRule type="notContainsBlanks" dxfId="120" priority="221">
+      <x:formula>LEN(TRIM(D19))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D19">
+    <x:cfRule type="cellIs" dxfId="119" priority="210" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="118" priority="120" operator="equal">
+    <x:cfRule type="cellIs" dxfId="118" priority="211" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D15:D16">
-    <x:cfRule type="cellIs" dxfId="117" priority="118" operator="equal">
+  <x:conditionalFormatting sqref="D19">
+    <x:cfRule type="cellIs" dxfId="117" priority="209" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D19">
-    <x:cfRule type="cellIs" dxfId="116" priority="108" operator="equal">
+  <x:conditionalFormatting sqref="A20:B20">
+    <x:cfRule type="cellIs" dxfId="116" priority="199" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="115" priority="109" operator="equal">
+    <x:cfRule type="cellIs" dxfId="115" priority="200" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="114" priority="110" operator="equal">
+    <x:cfRule type="cellIs" dxfId="114" priority="201" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="113" priority="111" operator="equal">
+    <x:cfRule type="cellIs" dxfId="113" priority="202" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="112" priority="112" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(D19,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="111" priority="113" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(D19,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="110" priority="114" operator="endsWith" text=" of">
-      <x:formula>RIGHT(D19,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="109" priority="115">
-      <x:formula>AND((RIGHT(D18, 3) = " of"), D20 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="108" priority="116">
-      <x:formula>AND(RIGHT(C19, 3) = " of", D20 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D19">
-    <x:cfRule type="notContainsBlanks" dxfId="107" priority="117">
-      <x:formula>LEN(TRIM(D19))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D19">
-    <x:cfRule type="cellIs" dxfId="106" priority="106" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="112" priority="203" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(A20,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="111" priority="204" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(A20,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="110" priority="205" operator="endsWith" text=" of">
+      <x:formula>RIGHT(A20,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="109" priority="206">
+      <x:formula>AND((RIGHT(A19, 3) = " of"), A21 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="108" priority="207">
+      <x:formula>AND(RIGHT(XFD20, 3) = " of", A21 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="A20:B20">
+    <x:cfRule type="notContainsBlanks" dxfId="107" priority="208">
+      <x:formula>LEN(TRIM(A20))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="A20:B20">
+    <x:cfRule type="cellIs" dxfId="106" priority="197" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="105" priority="107" operator="equal">
+    <x:cfRule type="cellIs" dxfId="105" priority="198" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D19">
-    <x:cfRule type="cellIs" dxfId="104" priority="105" operator="equal">
+  <x:conditionalFormatting sqref="A20:B20">
+    <x:cfRule type="cellIs" dxfId="104" priority="196" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="A20:B20">
-    <x:cfRule type="cellIs" dxfId="103" priority="95" operator="equal">
+  <x:conditionalFormatting sqref="A21:B24">
+    <x:cfRule type="cellIs" dxfId="103" priority="108" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="102" priority="96" operator="equal">
+    <x:cfRule type="cellIs" dxfId="102" priority="109" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="101" priority="97" operator="equal">
+    <x:cfRule type="cellIs" dxfId="101" priority="110" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="100" priority="98" operator="equal">
+    <x:cfRule type="cellIs" dxfId="100" priority="111" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="99" priority="99" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(A20,LEN("With Properties"))="With Properties"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="98" priority="100" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(A20,LEN(" table of"))=" table of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="97" priority="101" operator="endsWith" text=" of">
-      <x:formula>RIGHT(A20,LEN(" of"))=" of"</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="96" priority="102">
-      <x:formula>AND((RIGHT(A19, 3) = " of"), A21 = "With Properties")</x:formula>
-    </x:cfRule>
-    <x:cfRule type="expression" dxfId="95" priority="103">
-      <x:formula>AND(RIGHT(XFD20, 3) = " of", A21 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="A20:B20">
-    <x:cfRule type="notContainsBlanks" dxfId="94" priority="104">
-      <x:formula>LEN(TRIM(A20))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="A20:B20">
-    <x:cfRule type="cellIs" dxfId="93" priority="93" operator="equal">
+    <x:cfRule type="beginsWith" dxfId="99" priority="112" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(A21,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="98" priority="113" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(A21,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="97" priority="114" operator="endsWith" text=" of">
+      <x:formula>RIGHT(A21,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="96" priority="115">
+      <x:formula>AND((RIGHT(A20, 3) = " of"), A22 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="95" priority="116">
+      <x:formula>AND(RIGHT(XFD21, 3) = " of", A22 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="A21:B24">
+    <x:cfRule type="notContainsBlanks" dxfId="94" priority="117">
+      <x:formula>LEN(TRIM(A21))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="A21:B24">
+    <x:cfRule type="cellIs" dxfId="93" priority="106" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="92" priority="94" operator="equal">
+    <x:cfRule type="cellIs" dxfId="92" priority="107" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="A20:B20">
-    <x:cfRule type="cellIs" dxfId="91" priority="92" operator="equal">
+  <x:conditionalFormatting sqref="A21:B24">
+    <x:cfRule type="cellIs" dxfId="91" priority="105" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C20:D20">
-    <x:cfRule type="cellIs" dxfId="64" priority="56" operator="equal">
+  <x:conditionalFormatting sqref="A31:D34">
+    <x:cfRule type="cellIs" dxfId="90" priority="95" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="63" priority="57" operator="equal">
+    <x:cfRule type="cellIs" dxfId="89" priority="96" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="62" priority="58" operator="equal">
+    <x:cfRule type="cellIs" dxfId="88" priority="97" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="61" priority="59" operator="equal">
+    <x:cfRule type="cellIs" dxfId="87" priority="98" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="60" priority="60" operator="beginsWith" text="With Properties">
+    <x:cfRule type="beginsWith" dxfId="86" priority="99" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(A31,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="85" priority="100" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(A31,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="84" priority="101" operator="endsWith" text=" of">
+      <x:formula>RIGHT(A31,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="83" priority="102">
+      <x:formula>AND((RIGHT(A30, 3) = " of"), A32 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="82" priority="103">
+      <x:formula>AND(RIGHT(XFD31, 3) = " of", A32 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="A31:D34">
+    <x:cfRule type="notContainsBlanks" dxfId="81" priority="104">
+      <x:formula>LEN(TRIM(A31))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="A31:D34">
+    <x:cfRule type="cellIs" dxfId="80" priority="93" operator="equal">
+      <x:formula>"PercentagePrecision"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="cellIs" dxfId="79" priority="94" operator="equal">
+      <x:formula>"="</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="A31:D34">
+    <x:cfRule type="cellIs" dxfId="78" priority="92" operator="equal">
+      <x:formula>"StringFormat"</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="C23:C24">
+    <x:cfRule type="cellIs" dxfId="77" priority="82" operator="equal">
+      <x:formula>"Assert"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="cellIs" dxfId="76" priority="83" operator="equal">
+      <x:formula>"When"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="cellIs" dxfId="75" priority="84" operator="equal">
+      <x:formula>"Given a"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="cellIs" dxfId="74" priority="85" operator="equal">
+      <x:formula>"Specification"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="beginsWith" dxfId="73" priority="86" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(C23,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="72" priority="87" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(C23,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="71" priority="88" operator="endsWith" text=" of">
+      <x:formula>RIGHT(C23,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="70" priority="89">
+      <x:formula>AND((RIGHT(C22, 3) = " of"), C24 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="69" priority="90">
+      <x:formula>AND(RIGHT(B23, 3) = " of", C24 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="C23:C24">
+    <x:cfRule type="notContainsBlanks" dxfId="68" priority="91">
+      <x:formula>LEN(TRIM(C23))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="C23:C24">
+    <x:cfRule type="cellIs" dxfId="67" priority="80" operator="equal">
+      <x:formula>"PercentagePrecision"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="cellIs" dxfId="66" priority="81" operator="equal">
+      <x:formula>"="</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="C23:C24">
+    <x:cfRule type="cellIs" dxfId="65" priority="79" operator="equal">
+      <x:formula>"StringFormat"</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D23">
+    <x:cfRule type="cellIs" dxfId="64" priority="69" operator="equal">
+      <x:formula>"Assert"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="cellIs" dxfId="63" priority="70" operator="equal">
+      <x:formula>"When"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="cellIs" dxfId="62" priority="71" operator="equal">
+      <x:formula>"Given a"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="cellIs" dxfId="61" priority="72" operator="equal">
+      <x:formula>"Specification"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="beginsWith" dxfId="60" priority="73" operator="beginsWith" text="With Properties">
+      <x:formula>LEFT(D23,LEN("With Properties"))="With Properties"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="59" priority="74" operator="endsWith" text=" table of">
+      <x:formula>RIGHT(D23,LEN(" table of"))=" table of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="endsWith" dxfId="58" priority="75" operator="endsWith" text=" of">
+      <x:formula>RIGHT(D23,LEN(" of"))=" of"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="57" priority="76">
+      <x:formula>AND((RIGHT(D22, 3) = " of"), D24 = "With Properties")</x:formula>
+    </x:cfRule>
+    <x:cfRule type="expression" dxfId="56" priority="77">
+      <x:formula>AND(RIGHT(C23, 3) = " of", D24 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D23">
+    <x:cfRule type="notContainsBlanks" dxfId="55" priority="78">
+      <x:formula>LEN(TRIM(D23))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D23">
+    <x:cfRule type="cellIs" dxfId="54" priority="67" operator="equal">
+      <x:formula>"PercentagePrecision"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="cellIs" dxfId="53" priority="68" operator="equal">
+      <x:formula>"="</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D23">
+    <x:cfRule type="cellIs" dxfId="52" priority="66" operator="equal">
+      <x:formula>"StringFormat"</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="C20:D22">
+    <x:cfRule type="cellIs" dxfId="51" priority="56" operator="equal">
+      <x:formula>"Assert"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="cellIs" dxfId="50" priority="57" operator="equal">
+      <x:formula>"When"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="cellIs" dxfId="49" priority="58" operator="equal">
+      <x:formula>"Given a"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="cellIs" dxfId="48" priority="59" operator="equal">
+      <x:formula>"Specification"</x:formula>
+    </x:cfRule>
+    <x:cfRule type="beginsWith" dxfId="47" priority="60" operator="beginsWith" text="With Properties">
       <x:formula>LEFT(C20,LEN("With Properties"))="With Properties"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="59" priority="61" operator="endsWith" text=" table of">
+    <x:cfRule type="endsWith" dxfId="46" priority="61" operator="endsWith" text=" table of">
       <x:formula>RIGHT(C20,LEN(" table of"))=" table of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="58" priority="62" operator="endsWith" text=" of">
+    <x:cfRule type="endsWith" dxfId="45" priority="62" operator="endsWith" text=" of">
       <x:formula>RIGHT(C20,LEN(" of"))=" of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="57" priority="63">
+    <x:cfRule type="expression" dxfId="44" priority="63">
       <x:formula>AND((RIGHT(C19, 3) = " of"), C21 = "With Properties")</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="56" priority="64">
+    <x:cfRule type="expression" dxfId="43" priority="64">
       <x:formula>AND(RIGHT(B20, 3) = " of", C21 = "With Properties")</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C20:D20">
-    <x:cfRule type="notContainsBlanks" dxfId="55" priority="65">
+  <x:conditionalFormatting sqref="C20:D22">
+    <x:cfRule type="notContainsBlanks" dxfId="42" priority="65">
       <x:formula>LEN(TRIM(C20))&gt;0</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C20:D20">
-    <x:cfRule type="cellIs" dxfId="54" priority="54" operator="equal">
+  <x:conditionalFormatting sqref="C20:D22">
+    <x:cfRule type="cellIs" dxfId="41" priority="54" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="53" priority="55" operator="equal">
+    <x:cfRule type="cellIs" dxfId="40" priority="55" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="C20:D20">
-    <x:cfRule type="cellIs" dxfId="52" priority="53" operator="equal">
+  <x:conditionalFormatting sqref="C20:D22">
+    <x:cfRule type="cellIs" dxfId="39" priority="53" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D20">
-    <x:cfRule type="cellIs" dxfId="51" priority="43" operator="equal">
+  <x:conditionalFormatting sqref="D20:D21">
+    <x:cfRule type="cellIs" dxfId="38" priority="43" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="50" priority="44" operator="equal">
+    <x:cfRule type="cellIs" dxfId="37" priority="44" operator="equal">
       <x:formula>"When"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="49" priority="45" operator="equal">
+    <x:cfRule type="cellIs" dxfId="36" priority="45" operator="equal">
       <x:formula>"Given a"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="48" priority="46" operator="equal">
+    <x:cfRule type="cellIs" dxfId="35" priority="46" operator="equal">
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
-    <x:cfRule type="beginsWith" dxfId="47" priority="47" operator="beginsWith" text="With Properties">
+    <x:cfRule type="beginsWith" dxfId="34" priority="47" operator="beginsWith" text="With Properties">
       <x:formula>LEFT(D20,LEN("With Properties"))="With Properties"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="46" priority="48" operator="endsWith" text=" table of">
+    <x:cfRule type="endsWith" dxfId="33" priority="48" operator="endsWith" text=" table of">
       <x:formula>RIGHT(D20,LEN(" table of"))=" table of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="endsWith" dxfId="45" priority="49" operator="endsWith" text=" of">
+    <x:cfRule type="endsWith" dxfId="32" priority="49" operator="endsWith" text=" of">
       <x:formula>RIGHT(D20,LEN(" of"))=" of"</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="44" priority="50">
+    <x:cfRule type="expression" dxfId="31" priority="50">
       <x:formula>AND((RIGHT(D19, 3) = " of"), D21 = "With Properties")</x:formula>
     </x:cfRule>
-    <x:cfRule type="expression" dxfId="43" priority="51">
+    <x:cfRule type="expression" dxfId="30" priority="51">
       <x:formula>AND(RIGHT(C20, 3) = " of", D21 = "With Properties")</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D20">
-    <x:cfRule type="notContainsBlanks" dxfId="42" priority="52">
+  <x:conditionalFormatting sqref="D20:D21">
+    <x:cfRule type="notContainsBlanks" dxfId="29" priority="52">
       <x:formula>LEN(TRIM(D20))&gt;0</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D20">
-    <x:cfRule type="cellIs" dxfId="41" priority="41" operator="equal">
+  <x:conditionalFormatting sqref="D20:D21">
+    <x:cfRule type="cellIs" dxfId="28" priority="41" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
-    <x:cfRule type="cellIs" dxfId="40" priority="42" operator="equal">
+    <x:cfRule type="cellIs" dxfId="27" priority="42" operator="equal">
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="D20">
-    <x:cfRule type="cellIs" dxfId="39" priority="40" operator="equal">
+  <x:conditionalFormatting sqref="D20:D21">
+    <x:cfRule type="cellIs" dxfId="26" priority="40" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="A26:D29">
+  <x:conditionalFormatting sqref="D24">
     <x:cfRule type="cellIs" dxfId="25" priority="17" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
@@ -8275,27 +8446,27 @@
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
     <x:cfRule type="beginsWith" dxfId="21" priority="21" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(A26,LEN("With Properties"))="With Properties"</x:formula>
+      <x:formula>LEFT(D24,LEN("With Properties"))="With Properties"</x:formula>
     </x:cfRule>
     <x:cfRule type="endsWith" dxfId="20" priority="22" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(A26,LEN(" table of"))=" table of"</x:formula>
+      <x:formula>RIGHT(D24,LEN(" table of"))=" table of"</x:formula>
     </x:cfRule>
     <x:cfRule type="endsWith" dxfId="19" priority="23" operator="endsWith" text=" of">
-      <x:formula>RIGHT(A26,LEN(" of"))=" of"</x:formula>
+      <x:formula>RIGHT(D24,LEN(" of"))=" of"</x:formula>
     </x:cfRule>
     <x:cfRule type="expression" dxfId="18" priority="24">
-      <x:formula>AND((RIGHT(A25, 3) = " of"), A27 = "With Properties")</x:formula>
+      <x:formula>AND((RIGHT(D23, 3) = " of"), D25 = "With Properties")</x:formula>
     </x:cfRule>
     <x:cfRule type="expression" dxfId="17" priority="25">
-      <x:formula>AND(RIGHT(XFD26, 3) = " of", A27 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="A26:D29">
+      <x:formula>AND(RIGHT(C24, 3) = " of", D25 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D24">
     <x:cfRule type="notContainsBlanks" dxfId="16" priority="26">
-      <x:formula>LEN(TRIM(A26))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="A26:D29">
+      <x:formula>LEN(TRIM(D24))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="D24">
     <x:cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
@@ -8303,12 +8474,12 @@
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="A26:D29">
+  <x:conditionalFormatting sqref="D24">
     <x:cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="A21:D24">
+  <x:conditionalFormatting sqref="A26:D29">
     <x:cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <x:formula>"Assert"</x:formula>
     </x:cfRule>
@@ -8322,27 +8493,27 @@
       <x:formula>"Specification"</x:formula>
     </x:cfRule>
     <x:cfRule type="beginsWith" dxfId="8" priority="8" operator="beginsWith" text="With Properties">
-      <x:formula>LEFT(A21,LEN("With Properties"))="With Properties"</x:formula>
+      <x:formula>LEFT(A26,LEN("With Properties"))="With Properties"</x:formula>
     </x:cfRule>
     <x:cfRule type="endsWith" dxfId="7" priority="9" operator="endsWith" text=" table of">
-      <x:formula>RIGHT(A21,LEN(" table of"))=" table of"</x:formula>
+      <x:formula>RIGHT(A26,LEN(" table of"))=" table of"</x:formula>
     </x:cfRule>
     <x:cfRule type="endsWith" dxfId="6" priority="10" operator="endsWith" text=" of">
-      <x:formula>RIGHT(A21,LEN(" of"))=" of"</x:formula>
+      <x:formula>RIGHT(A26,LEN(" of"))=" of"</x:formula>
     </x:cfRule>
     <x:cfRule type="expression" dxfId="5" priority="11">
-      <x:formula>AND((RIGHT(A20, 3) = " of"), A22 = "With Properties")</x:formula>
+      <x:formula>AND((RIGHT(A25, 3) = " of"), A27 = "With Properties")</x:formula>
     </x:cfRule>
     <x:cfRule type="expression" dxfId="4" priority="12">
-      <x:formula>AND(RIGHT(XFD21, 3) = " of", A22 = "With Properties")</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="A21:D24">
+      <x:formula>AND(RIGHT(XFD26, 3) = " of", A27 = "With Properties")</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="A26:D29">
     <x:cfRule type="notContainsBlanks" dxfId="3" priority="13">
-      <x:formula>LEN(TRIM(A21))&gt;0</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="A21:D24">
+      <x:formula>LEN(TRIM(A26))&gt;0</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="A26:D29">
     <x:cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <x:formula>"PercentagePrecision"</x:formula>
     </x:cfRule>
@@ -8350,7 +8521,7 @@
       <x:formula>"="</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="A21:D24">
+  <x:conditionalFormatting sqref="A26:D29">
     <x:cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <x:formula>"StringFormat"</x:formula>
     </x:cfRule>

</xml_diff>

<commit_message>
Fix date format in excel
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/PrimitiveLists.xlsx
+++ b/SampleTests/ExcelTests/PrimitiveLists.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\SampleTests\ExcelTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886E834E-BAB7-456D-B19D-323D89533D02}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A668CF4A-A5D7-4AB2-919B-19DEA64083AE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{93574C7F-CD34-4A26-A791-2CAAC18DAAC8}"/>
   </bookViews>
@@ -143,7 +143,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -179,7 +179,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -602,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07917FFE-3CF1-4F24-ADDD-99FADF944328}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,7 +613,7 @@
     <col min="3" max="3" width="28.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="60" style="1" customWidth="1"/>
     <col min="8" max="8" width="36.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="1"/>
@@ -880,7 +880,7 @@
       <c r="E42" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F42" s="2">
         <v>43833</v>
       </c>
     </row>
@@ -893,7 +893,7 @@
       <c r="E44" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F44" s="1">
+      <c r="F44" s="2">
         <v>43834</v>
       </c>
     </row>

</xml_diff>